<commit_message>
Adding alternative search if not Elasticsearch connected and fixing errors
</commit_message>
<xml_diff>
--- a/content.xlsx
+++ b/content.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="languages" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="240">
   <si>
     <t xml:space="preserve">language</t>
   </si>
@@ -172,6 +172,42 @@
     <t xml:space="preserve">Keywords</t>
   </si>
   <si>
+    <t xml:space="preserve">search</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type &amp; Hit Enter to search projects…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">search_keyw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Search keywords...</t>
+  </si>
+  <si>
+    <t xml:space="preserve">error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Something went wrong</t>
+  </si>
+  <si>
+    <t xml:space="preserve">error_subtitle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We have taken note of the error and will try to fix it as soon as possible.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">back_home</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Back To Home</t>
+  </si>
+  <si>
+    <t xml:space="preserve">404_error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">404 Page Not Found!</t>
+  </si>
+  <si>
     <t xml:space="preserve">Inicio</t>
   </si>
   <si>
@@ -238,6 +274,24 @@
     <t xml:space="preserve">lectura</t>
   </si>
   <si>
+    <t xml:space="preserve">Escribe y pulsa Enter para buscar projectos…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buscar palabras clave…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Algo ha ido mal.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hemos tomado nota del error, lo intentaremos solucionar lo antes posible.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Volver A Inicio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">404 Página no encontrada!</t>
+  </si>
+  <si>
     <t xml:space="preserve">index</t>
   </si>
   <si>
@@ -286,36 +340,9 @@
     <t xml:space="preserve">parragraph3</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Then, when my youngest baby was ready to be born I had the chance to join [**Ironhack**](</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">https://www.ironhack.com/es/en/data-analytics/remote</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">) to improve my skills of data mining and learn much more about analysis and artificial intelligence. 
+    <t xml:space="preserve">Then, when my youngest baby was ready to be born I had the chance to join [**Ironhack**](https://www.ironhack.com/es/en/data-analytics/remote) to improve my skills of data mining and learn much more about analysis and artificial intelligence. 
 During this time I had to face many challenges that the teaching team provided us which I could solve, making me feel more confident with my skills and learning and creating projects (like my final project, Ironhack repository) that could help others to improve their skills too.
 </t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">parragraph4</t>
@@ -848,7 +875,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -873,8 +900,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -962,12 +997,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="bottomLeft" activeCell="D53" activeCellId="0" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1235,245 +1270,383 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="4" t="s">
-        <v>6</v>
+      <c r="B24" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>49</v>
+        <v>1</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="1" t="s">
-        <v>8</v>
+        <v>51</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>50</v>
+        <v>1</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="4" t="s">
-        <v>10</v>
+      <c r="B26" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>51</v>
+        <v>1</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="4" t="s">
-        <v>12</v>
+      <c r="B27" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>52</v>
+        <v>1</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="4" t="s">
-        <v>14</v>
+      <c r="B28" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>53</v>
+        <v>1</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="4" t="s">
-        <v>16</v>
+      <c r="B29" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>54</v>
+        <v>1</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="4" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D30" s="4" t="s">
-        <v>55</v>
+      <c r="D30" s="7" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="4" t="s">
-        <v>20</v>
+      <c r="B31" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="4" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="4" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="4" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="4" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="4" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="4" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="4" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="4" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="4" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C41" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="1" t="s">
+      <c r="C47" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B48" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B43" s="4" t="s">
+      <c r="C48" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B49" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C43" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B44" s="4" t="s">
+      <c r="C49" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B50" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C44" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B45" s="4" t="s">
+      <c r="C50" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B51" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C45" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D45" s="6" t="s">
-        <v>70</v>
+      <c r="C51" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="52" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="5"/>
+      <c r="B52" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="53" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="5"/>
+      <c r="B53" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="54" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="5"/>
+      <c r="B54" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="55" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="5"/>
+      <c r="B55" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="56" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="5"/>
+      <c r="B56" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="57" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="5"/>
+      <c r="B57" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D57" s="6" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1494,8 +1667,8 @@
   </sheetPr>
   <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
@@ -1507,7 +1680,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="124.9"/>
   </cols>
   <sheetData>
-    <row r="1" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -1523,178 +1696,178 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>71</v>
+        <v>89</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>72</v>
+        <v>90</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>73</v>
+      <c r="D2" s="10" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>71</v>
+        <v>89</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>74</v>
+        <v>92</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>75</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>71</v>
+        <v>89</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>76</v>
+        <v>94</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>77</v>
+      <c r="D4" s="10" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>71</v>
+        <v>89</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>72</v>
+        <v>90</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="8" t="s">
-        <v>78</v>
+      <c r="D5" s="10" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>71</v>
+        <v>89</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>74</v>
+        <v>92</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>75</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>71</v>
+        <v>89</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>76</v>
+        <v>94</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="8" t="s">
-        <v>79</v>
+      <c r="D7" s="10" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>72</v>
+        <v>90</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="8" t="s">
-        <v>81</v>
+      <c r="D8" s="10" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>82</v>
+        <v>100</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>83</v>
+      <c r="D9" s="10" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>84</v>
+        <v>102</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="8" t="s">
-        <v>85</v>
+      <c r="D10" s="10" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>86</v>
+        <v>104</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="8" t="s">
-        <v>87</v>
+      <c r="D11" s="11" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>88</v>
+        <v>106</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="8" t="s">
-        <v>89</v>
+      <c r="D12" s="10" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>90</v>
+        <v>108</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="8" t="s">
-        <v>91</v>
+      <c r="D13" s="10" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>1</v>
@@ -1702,164 +1875,164 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D15" s="8" t="s">
-        <v>94</v>
+      <c r="D15" s="10" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>95</v>
+        <v>113</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D16" s="8" t="s">
-        <v>96</v>
+      <c r="D16" s="10" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D17" s="8" t="s">
-        <v>98</v>
+      <c r="D17" s="10" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>99</v>
+        <v>117</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D18" s="8" t="s">
-        <v>100</v>
+      <c r="D18" s="10" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>101</v>
+        <v>119</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D19" s="9" t="s">
-        <v>102</v>
+      <c r="D19" s="11" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>72</v>
+        <v>90</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D20" s="8" t="s">
-        <v>103</v>
+      <c r="D20" s="10" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>82</v>
+        <v>100</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D21" s="8" t="s">
-        <v>104</v>
+      <c r="D21" s="10" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>84</v>
+        <v>102</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D22" s="8" t="s">
-        <v>105</v>
+      <c r="D22" s="10" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>86</v>
+        <v>104</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D23" s="8" t="s">
-        <v>106</v>
+      <c r="D23" s="10" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>88</v>
+        <v>106</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D24" s="8" t="s">
-        <v>107</v>
+      <c r="D24" s="10" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>90</v>
+        <v>108</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D25" s="8" t="s">
-        <v>108</v>
+      <c r="D25" s="10" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>2</v>
@@ -1867,301 +2040,301 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="8" t="s">
-        <v>109</v>
+      <c r="D27" s="10" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>95</v>
+        <v>113</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D28" s="8" t="s">
-        <v>110</v>
+      <c r="D28" s="10" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D29" s="8" t="s">
-        <v>111</v>
+      <c r="D29" s="10" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>99</v>
+        <v>117</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D30" s="8" t="s">
-        <v>112</v>
+      <c r="D30" s="10" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>101</v>
+        <v>119</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D31" s="9" t="s">
-        <v>102</v>
+      <c r="D31" s="11" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>113</v>
+        <v>131</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>114</v>
+        <v>132</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D32" s="8" t="s">
-        <v>115</v>
+      <c r="D32" s="10" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>113</v>
+        <v>131</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>76</v>
+        <v>94</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D33" s="8" t="s">
-        <v>116</v>
+      <c r="D33" s="10" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>113</v>
+        <v>131</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>117</v>
+        <v>135</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D34" s="8" t="s">
-        <v>118</v>
+      <c r="D34" s="10" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>113</v>
+        <v>131</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>119</v>
+        <v>137</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D35" s="8" t="s">
-        <v>120</v>
+      <c r="D35" s="10" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>113</v>
+        <v>131</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>121</v>
+        <v>139</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D36" s="8" t="s">
-        <v>122</v>
+      <c r="D36" s="10" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>113</v>
+        <v>131</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>123</v>
+        <v>141</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D37" s="8" t="s">
-        <v>124</v>
+      <c r="D37" s="10" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>113</v>
+        <v>131</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>125</v>
+        <v>143</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D38" s="8" t="s">
-        <v>126</v>
+      <c r="D38" s="10" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>113</v>
+        <v>131</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>127</v>
+        <v>145</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D39" s="8" t="s">
-        <v>128</v>
+      <c r="D39" s="10" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>113</v>
+        <v>131</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>114</v>
+        <v>132</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D40" s="8" t="s">
-        <v>129</v>
+      <c r="D40" s="10" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>113</v>
+        <v>131</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>76</v>
+        <v>94</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D41" s="8" t="s">
-        <v>130</v>
+      <c r="D41" s="10" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>113</v>
+        <v>131</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>117</v>
+        <v>135</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D42" s="8" t="s">
-        <v>131</v>
+      <c r="D42" s="10" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>113</v>
+        <v>131</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>119</v>
+        <v>137</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D43" s="8" t="s">
-        <v>132</v>
+      <c r="D43" s="10" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>113</v>
+        <v>131</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>121</v>
+        <v>139</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D44" s="8" t="s">
-        <v>133</v>
+      <c r="D44" s="10" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>113</v>
+        <v>131</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>123</v>
+        <v>141</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D45" s="8" t="s">
-        <v>134</v>
+      <c r="D45" s="10" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>113</v>
+        <v>131</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>125</v>
+        <v>143</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D46" s="8" t="s">
-        <v>135</v>
+      <c r="D46" s="10" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>113</v>
+        <v>131</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>127</v>
+        <v>145</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D47" s="8" t="s">
-        <v>136</v>
+      <c r="D47" s="10" t="s">
+        <v>154</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D11" r:id="rId1" display="https://www.ironhack.com/es/en/data-analytics/remote"/>
+    <hyperlink ref="D11" r:id="rId1" display="Then, when my youngest baby was ready to be born I had the chance to join [**Ironhack**](https://www.ironhack.com/es/en/data-analytics/remote) to improve my skills of data mining and learn much more about analysis and artificial intelligence. &#10;During this time I had to face many challenges that the teaching team provided us which I could solve, making me feel more confident with my skills and learning and creating projects (like my final project, Ironhack repository) that could help others to improve their skills too.&#10;"/>
     <hyperlink ref="D19" r:id="rId2" display="https://www.youtube.com/embed/8CAoLz4NS5o"/>
     <hyperlink ref="D31" r:id="rId3" display="https://www.youtube.com/embed/8CAoLz4NS5o"/>
   </hyperlinks>
@@ -2185,12 +2358,12 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
+      <selection pane="bottomLeft" activeCell="H27" activeCellId="0" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="10" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="12" width="11.53"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="11.53"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="24.66"/>
@@ -2200,60 +2373,60 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="24" min="9" style="1" width="11.53"/>
   </cols>
   <sheetData>
-    <row r="1" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>138</v>
+    <row r="1" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>156</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>114</v>
+        <v>132</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>139</v>
+        <v>157</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>140</v>
+        <v>158</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>141</v>
+        <v>159</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>142</v>
+        <v>160</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>143</v>
+        <v>161</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>144</v>
+        <v>162</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>145</v>
+        <v>163</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>146</v>
+        <v>164</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>147</v>
+        <v>165</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>148</v>
+        <v>166</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>149</v>
+        <v>167</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>150</v>
+        <v>168</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>151</v>
+        <v>169</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>152</v>
+        <v>170</v>
       </c>
       <c r="S1" s="2"/>
       <c r="T1" s="2"/>
@@ -2263,444 +2436,444 @@
       <c r="X1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="11" t="n">
+      <c r="A2" s="13" t="n">
         <v>44910</v>
       </c>
-      <c r="B2" s="10" t="n">
+      <c r="B2" s="12" t="n">
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>153</v>
+        <v>171</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>154</v>
+        <v>172</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>155</v>
+        <v>173</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>156</v>
+        <v>174</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>157</v>
+        <v>175</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>158</v>
+        <v>176</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>159</v>
+        <v>177</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>159</v>
+        <v>177</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>151</v>
+        <v>169</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>152</v>
+        <v>170</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="11" t="n">
+      <c r="A3" s="13" t="n">
         <v>44910</v>
       </c>
-      <c r="B3" s="10" t="n">
+      <c r="B3" s="12" t="n">
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>153</v>
+        <v>171</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>160</v>
+        <v>178</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>161</v>
+        <v>179</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>162</v>
+        <v>180</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>163</v>
+        <v>181</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>158</v>
+        <v>176</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>159</v>
+        <v>177</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>159</v>
+        <v>177</v>
       </c>
       <c r="Q3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="11" t="n">
+      <c r="A4" s="13" t="n">
         <v>44986</v>
       </c>
-      <c r="B4" s="10" t="n">
+      <c r="B4" s="12" t="n">
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>164</v>
+        <v>182</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>165</v>
+        <v>183</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>166</v>
+        <v>184</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>167</v>
+        <v>185</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>168</v>
+        <v>186</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>169</v>
+        <v>187</v>
       </c>
       <c r="O4" s="5" t="s">
-        <v>170</v>
+        <v>188</v>
       </c>
       <c r="P4" s="5" t="s">
-        <v>170</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="11" t="n">
+      <c r="A5" s="13" t="n">
         <v>44986</v>
       </c>
-      <c r="B5" s="12" t="n">
+      <c r="B5" s="14" t="n">
         <v>1</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>164</v>
+        <v>182</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>171</v>
+        <v>189</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>172</v>
+        <v>190</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>173</v>
+        <v>191</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>169</v>
+        <v>187</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>170</v>
+        <v>188</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>170</v>
+        <v>188</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="11" t="n">
+      <c r="A6" s="13" t="n">
         <v>45017</v>
       </c>
-      <c r="B6" s="10" t="n">
+      <c r="B6" s="12" t="n">
         <v>1</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>175</v>
+        <v>193</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>176</v>
+        <v>194</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>177</v>
+        <v>195</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>178</v>
+        <v>196</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>179</v>
+        <v>197</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>180</v>
+        <v>198</v>
       </c>
       <c r="L6" s="5"/>
       <c r="O6" s="5" t="s">
-        <v>181</v>
+        <v>199</v>
       </c>
       <c r="P6" s="5" t="s">
-        <v>181</v>
+        <v>199</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="11" t="n">
+      <c r="A7" s="13" t="n">
         <v>45017</v>
       </c>
-      <c r="B7" s="10" t="n">
+      <c r="B7" s="12" t="n">
         <v>1</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>182</v>
+        <v>200</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>183</v>
+        <v>201</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>184</v>
+        <v>202</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>185</v>
+        <v>203</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>186</v>
+        <v>204</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>180</v>
+        <v>198</v>
       </c>
       <c r="L7" s="5"/>
       <c r="O7" s="1" t="s">
-        <v>181</v>
+        <v>199</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>181</v>
+        <v>199</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="11" t="n">
+      <c r="A8" s="13" t="n">
         <v>45047</v>
       </c>
-      <c r="B8" s="10" t="n">
+      <c r="B8" s="12" t="n">
         <v>1</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>187</v>
+        <v>205</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>188</v>
+        <v>206</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>189</v>
+        <v>207</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>190</v>
+        <v>208</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>191</v>
+        <v>209</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>192</v>
+        <v>210</v>
       </c>
       <c r="O8" s="5" t="s">
-        <v>193</v>
+        <v>211</v>
       </c>
       <c r="P8" s="5" t="s">
-        <v>193</v>
+        <v>211</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="11" t="n">
+      <c r="A9" s="13" t="n">
         <v>45047</v>
       </c>
-      <c r="B9" s="10" t="n">
+      <c r="B9" s="12" t="n">
         <v>1</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>194</v>
+        <v>212</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>195</v>
+        <v>213</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>196</v>
+        <v>214</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>197</v>
+        <v>215</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>198</v>
+        <v>216</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>192</v>
+        <v>210</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>193</v>
+        <v>211</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>193</v>
+        <v>211</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="11" t="n">
+      <c r="A10" s="13" t="n">
         <v>45078</v>
       </c>
-      <c r="B10" s="10" t="n">
+      <c r="B10" s="12" t="n">
         <v>1</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="O10" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="P10" s="5" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="13" t="n">
+        <v>45078</v>
+      </c>
+      <c r="B11" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="O11" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="P11" s="5" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="11.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="13" t="n">
+        <v>45170</v>
+      </c>
+      <c r="B12" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="O12" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="P12" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="O10" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="P10" s="5" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="11" t="n">
-        <v>45078</v>
-      </c>
-      <c r="B11" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="O11" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="P11" s="5" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="11.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="11" t="n">
+      <c r="Q12" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="R12" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="13" t="n">
         <v>45170</v>
       </c>
-      <c r="B12" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="E12" s="1" t="s">
+      <c r="B13" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="O13" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="P13" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q13" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="F12" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="O12" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="P12" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="Q12" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="R12" s="1" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="11" t="n">
-        <v>45170</v>
-      </c>
-      <c r="B13" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>218</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>219</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>220</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="O13" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="P13" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="Q13" s="1" t="s">
-        <v>193</v>
-      </c>
       <c r="R13" s="1" t="s">
-        <v>204</v>
+        <v>222</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Fixing errors in the project details
</commit_message>
<xml_diff>
--- a/content.xlsx
+++ b/content.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="languages" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="244">
   <si>
     <t xml:space="preserve">language</t>
   </si>
@@ -542,37 +542,58 @@
     <t xml:space="preserve">image3</t>
   </si>
   <si>
-    <t xml:space="preserve">Lyrics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resume1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Description1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Action1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">resolution1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Keyword1, Keyword2, Keyword3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lyrics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resumen1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Acción1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">resolución1</t>
+    <t xml:space="preserve">One story about Life Expectancy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How has Life Expectancy evolved over the years in the world? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I was asked to create one dashboard using [**Tableau**](https://www.tableau.com/) and collecting the data wherever I wanted. So I decided to go for *one story about Life Expectancy* but trying to look at the data from a different perspective than the usual GDP or any economic reasons.
+&lt;img&gt;image1&lt;/img&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Firstly I was researching the different sources that I could use to create my database, since I wanted to analyze a Life Expectancy over many years it was not easy find different databases with the required information. At the end I decided to use [*The World Bank*](https://www.worldbank.org/en/home) databases so I spend quite amount of time digging in that databases.  
+When I downloaded all the interesting databases for my project (not all were useful), I had to process them with **python** to normalize the data and prepare one only database to use in **Tableau**.  
+The path since I started to create the dashboard brought to the front how the human nature could affect the Life Expectancy, for instance the &lt;u&gt;genocides&lt;/u&gt; or the &lt;u&gt;basic sanitation services&lt;/u&gt;.
+I tried to show the information like a *story*, starting in the year 1960 and finishing in the year 2020, unfortunately the information didn't include the *pandemic of Covid* but I think that could be a little bit interesting all I could show in my dashboard like the Life Expectancy changing or the deviation from the mean in the 2020 year.  
+&lt;img&gt;image2&lt;/img&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">So, if you want to see the result of this project, you can go to [**One story about Life Expectancy**](https://public.tableau.com/views/TableauProject_16693794082020/Presentation?:language=en-US&amp;:display_count=n&amp;:origin=viz_share_link)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tableau, visualization, dashboard, python</t>
+  </si>
+  <si>
+    <t xml:space="preserve">project0101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">project0102</t>
+  </si>
+  <si>
+    <t xml:space="preserve">project0103</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Una historia sobre Esperanza de Vida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">¿Cómo ha evolucionado la Esperanza de Vida a lo largo de los años en el mundo?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Me pidieron que creara una presentación usando [**Tableau**](https://www.tableau.com/) recopilando los datos donde quisiera. Así que decidí buscar *una historia sobre Esperanza de Vida* pero tratando de ver los datos desde una perspectiva diferente a la del PIB habitual o cualquier razón económica. 
+&lt;img&gt;image1&lt;/img&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Primero estuve investigando las diferentes fuentes que podía utilizar para crear mi base de datos, ya que quería analizar la Esperanza de Vida a lo largo de muchos años no era fácil encontrar diferentes bases de datos con la información requerida. Al final decidí utilizar las bases de datos de [*The World Bank*](https://www.worldbank.org/en/home) así que dediqué bastante tiempo a investigar más en profundidad dichas bases datos.  
+Cuando descargué todas las bases de datos que consideré interesantes para mi proyecto (no todas eran útiles), tuve que procesarlas con **python** para normalizar los datos y preparar una única base de datos para usarla en **Tableau**.  
+El camino desde que comencé a crear el tablero sacó a relucir cómo la naturaleza humana podría afectar a la Esperanza de Vida, por ejemplo los  &lt;u&gt;genocidios&lt;/u&gt; o los &lt;u&gt;servicios básicos de saneamiento&lt;/u&gt;.  
+Intenté mostrar la información como un *historia*, empezando en el año 1960 y terminando en el año 2020, lamentablemente la información no incluía la *pandemia del Covid*  pero creo que podría ser un poco interesante todo lo que pude mostrar en my tablero como el cambio en la Esperanza de Vida o la desviación de la media en el año 2020.  &lt;img&gt;image2&lt;/img&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Así que, si quieres ver el resultado de este proyecto, puedes ir a [**Una historia sobre Esperanza de Vida**](https://public.tableau.com/views/TableauProject_16693794082020/Presentation?:language=en-US&amp;:display_count=n&amp;:origin=viz_share_link)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tableau, visualización, dashboard, python</t>
   </si>
   <si>
     <t xml:space="preserve">IronHack Repository</t>
@@ -783,7 +804,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -830,6 +851,13 @@
       <color rgb="FF0000FF"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -908,7 +936,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -932,7 +960,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -999,7 +1027,7 @@
   </sheetPr>
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="D53" activeCellId="0" sqref="D53"/>
@@ -2355,17 +2383,17 @@
   </sheetPr>
   <dimension ref="A1:X25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="H27" activeCellId="0" sqref="H27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="12" width="11.53"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="11.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="28.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="24.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="43.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="19.6"/>
@@ -2435,9 +2463,9 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="650.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="13" t="n">
-        <v>44910</v>
+        <v>44890</v>
       </c>
       <c r="B2" s="12" t="n">
         <v>1</v>
@@ -2451,13 +2479,13 @@
       <c r="E2" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="14" t="s">
         <v>175</v>
       </c>
       <c r="I2" s="1" t="s">
@@ -2467,50 +2495,49 @@
         <v>177</v>
       </c>
       <c r="P2" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="13" t="n">
+        <v>44890</v>
+      </c>
+      <c r="B3" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="O3" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="Q2" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="13" t="n">
-        <v>44910</v>
-      </c>
-      <c r="B3" s="12" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="P3" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="Q3" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="Q3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="13" t="n">
@@ -2523,63 +2550,63 @@
         <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="O4" s="5" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="P4" s="5" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="13" t="n">
         <v>44986</v>
       </c>
-      <c r="B5" s="14" t="n">
+      <c r="B5" s="8" t="n">
         <v>1</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="G5" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="O5" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="I5" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="P5" s="1" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2593,29 +2620,29 @@
         <v>1</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="L6" s="5"/>
       <c r="O6" s="5" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="P6" s="5" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2629,29 +2656,29 @@
         <v>2</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="F7" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>202</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>198</v>
       </c>
       <c r="L7" s="5"/>
       <c r="O7" s="1" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2665,28 +2692,28 @@
         <v>1</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="O8" s="5" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="P8" s="5" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2700,28 +2727,28 @@
         <v>2</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="F9" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="O9" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="O9" s="1" t="s">
-        <v>211</v>
-      </c>
       <c r="P9" s="1" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2735,28 +2762,28 @@
         <v>1</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>161</v>
       </c>
       <c r="O10" s="5" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="P10" s="5" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2770,28 +2797,28 @@
         <v>2</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="I11" s="5" t="s">
         <v>161</v>
       </c>
       <c r="O11" s="5" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="P11" s="5" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="11.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2805,34 +2832,34 @@
         <v>1</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="O12" s="5" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="P12" s="5" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2846,34 +2873,34 @@
         <v>2</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="H13" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="O13" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="I13" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="O13" s="3" t="s">
-        <v>234</v>
-      </c>
       <c r="P13" s="5" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2883,6 +2910,10 @@
       <c r="L25" s="5"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1" display="So, if you want to see the result of this project, you can go to [**One story about Life Expectancy**](https://public.tableau.com/views/TableauProject_16693794082020/Presentation?:language=en-US&amp;:display_count=n&amp;:origin=viz_share_link)"/>
+    <hyperlink ref="H3" r:id="rId2" display="Así que, si quieres ver el resultado de este proyecto, puedes ir a [**Una historia sobre Esperanza de Vida**](https://public.tableau.com/views/TableauProject_16693794082020/Presentation?:language=en-US&amp;:display_count=n&amp;:origin=viz_share_link)"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Readme and the last improvements
</commit_message>
<xml_diff>
--- a/content.xlsx
+++ b/content.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="221">
   <si>
     <t xml:space="preserve">language</t>
   </si>
@@ -548,14 +548,14 @@
     <t xml:space="preserve">How has Life Expectancy evolved over the years in the world? </t>
   </si>
   <si>
-    <t xml:space="preserve">I was asked to create one dashboard using [**Tableau**](https://www.tableau.com/) and collecting the data wherever I wanted. So I decided to go for *one story about Life Expectancy* but trying to look at the data from a different perspective than the usual GDP or any economic reasons.
+    <t xml:space="preserve">I was asked to create one dashboard using [**Tableau**](https://www.tableau.com/) and collect the data wherever I wanted. So I decided to go for *one story about Life Expectancy* but try to look at the data from a different perspective than the usual GDP or any economic reasons.  
 &lt;img&gt;image1&lt;/img&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Firstly I was researching the different sources that I could use to create my database, since I wanted to analyze a Life Expectancy over many years it was not easy find different databases with the required information. At the end I decided to use [*The World Bank*](https://www.worldbank.org/en/home) databases so I spend quite amount of time digging in that databases.  
-When I downloaded all the interesting databases for my project (not all were useful), I had to process them with **python** to normalize the data and prepare one only database to use in **Tableau**.  
-The path since I started to create the dashboard brought to the front how the human nature could affect the Life Expectancy, for instance the &lt;u&gt;genocides&lt;/u&gt; or the &lt;u&gt;basic sanitation services&lt;/u&gt;.
-I tried to show the information like a *story*, starting in the year 1960 and finishing in the year 2020, unfortunately the information didn't include the *pandemic of Covid* but I think that could be a little bit interesting all I could show in my dashboard like the Life Expectancy changing or the deviation from the mean in the 2020 year.  
+    <t xml:space="preserve">Firstly I researched the different sources that I could use to create my database, since I wanted to analyze Life Expectancy over many years it was not easy to find different databases with the required information. In the end, I decided to use [*The World Bank*](https://www.worldbank.org/en/home) databases so I spent quite an amount of time digging into those databases.   
+When I downloaded all the interesting databases for my project (not all were useful), I had to process them with **python** to normalize the data and prepare one only database to use in **Tableau**.   
+The path since I started to create the dashboard brought to the front how human nature could affect Life Expectancy, for instance, the &lt;u&gt;genocides&lt;/u&gt; or the &lt;u&gt;basic sanitation services&lt;/u&gt;.  
+I tried to show the information like a *story*, starting in the year 1960 and finishing in the year 2020, unfortunately, the information didn't include the *pandemic of Covid* but I think that could be a little bit interesting all I could show in my dashboard like the Life Expectancy changing or the deviation from the mean in the 2020 year.   
 &lt;img&gt;image2&lt;/img&gt;</t>
   </si>
   <si>
@@ -596,203 +596,316 @@
     <t xml:space="preserve">tableau, visualización, dashboard, python</t>
   </si>
   <si>
-    <t xml:space="preserve">IronHack Repository</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resume2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Description2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Action2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">resolution2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Keyword1, Keyword4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ihrep</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resumen2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Acción2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">resolución2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Project 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resume3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Description3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Action3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">resolution3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Keyword</t>
-  </si>
-  <si>
-    <t xml:space="preserve">project04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proyecto 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resumen3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">acción3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">resolución3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Project 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resume4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Description4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Action4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">resolution4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Keyword4, Keyword3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">project05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proyecto 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resumen4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Acción4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">resolución4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Project 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resume5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Description5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Action5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">resolution5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">project06</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proyecto 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resumen5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Acción5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">resolución5</t>
+    <t xml:space="preserve">Lyrics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What do the songs talk about? What is the sentiment of their lyrics? And what about the genres or the artists? This project tries to shed some light on this and other questions.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is the project that I created for my Mid-Bootcamp task in [IronHack](http://www.ironhack.com).     
+I had some requirements and restrictions like:     
+1. Collect the data by myself (cannot download datasets)  
+2. The dataset should have between 30 and 100 observations (rows) and 5 to 10 features (columns)  
+3. I could enrich the dataset with more information obtained with other methods than manual typing (for example, web scraping)  4. Need to complete one analysis to answer the questions that I have to solve with this project, also I should supplement the analysis with some hypothesis.     
+##### My project   
+My questions were about the lyrics of the songs that we use to listen every day, these questions are:     
+1. Do the lyrics have an overall positive sentiment?  
+2. Are women's lyrics more positive than men's  
+3. Are pop's lyrics better than hip hop's?     
+&lt;img&gt;image1&lt;/img&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">##### My solution     
+###### Python      
+- Creation of the dataset using Python:   
+I decided to collect information from [Spotify Charts](https://charts.spotify.com/) because I wanted to analyze lyrics globally, so I chose the top artist of week 47 of the year 2022. The process I followed was to type in a file the artist of that chart and also use [Last.fm](https://www.last.fm/) to type more information like gender, main genre and if is a band.  
+Then I complete the dataset by searching the 10 most popular songs of every artist in [Spotify](https://open.spotify.com/) using their API.   
+After that, I used the [__lyricsgenius__](https://pypi.org/project/lyricsgenius/) library to connect to the website [Genius](https://genius.com/) to download 5 lyrics of the 10 most popular songs in Spotify of every artist (because the name of the songs in Spotify not always has a corresponding name in Genius).   
+At this point, I also created one function with [Selenium](https://www.selenium.dev/) to get the connection token, just in case the token to connect to Genius changes.   
+Right now is stored in a file (secrets.txt) but could get it without storing it.   
+&lt;img&gt;image2&lt;/img&gt;  
+- Sentiment Analysis:   
+Once I downloaded all the information, needed to make a treatment to do the sentiment analysis (using the library [__Flair__](https://github.com/flairNLP/flair)) and natural language processing ([__NLTK__](https://www.nltk.org/)).  
+- Translations:   
+Since the list of songs was used in different languages, I decided to translate all into English to simplify the analysis. For this, I used the library [__Fasttext__](https://fasttext.cc/) with their pre-trained model to detect the language of the lyrics and then translate them to English with the library [__translators__](https://github.com/uliontse/translators) which if cannot do the translation uses google translator to perform the work.   
+- Top words:   
+I calculated the top words with NLTK functions and update manually their stop words list to include more that where not interesting to my analysis.  
+- Wordcloud:   
+I also created a function to generate a one-word cloud with the library __wordcloud__ and __PIL__ to show different shapes that I downloaded.  
+- Hypothesis analysis:   
+In another Jupyter notebook, I developed the hypothesis analysis and prepared the dataset for the visual analysis with [Tableau](https://public.tableau.com/)    
+###### Tableau   
+I used Tableau in his public version to create the presentation of the project and the visual analysis of the project, which can be found in [_my Tableau_](https://public.tableau.com/app/profile/.scar.iglesias.roqueiro/viz/Mid-BootcampProject_16711135428210/Lyrics)     
+&lt;img&gt;image3&lt;/img&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">To summarize the links of my project, here they are:  
+- Presentation video: [__My Youtube__](https://youtu.be/Veu5M7_hCUg)  
+- Visualizations: [__My Tableau__](https://public.tableau.com/app/profile/.scar.iglesias.roqueiro/viz/Mid-BootcampProject_16711135428210/Lyrics)  
+- Source codes (including the Flask App): [__My Github__](https://github.com/oiroqueiro/mid-bootcamp-project)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tableau, visualization, dashboard, python, flask, web scrapping, API, Selenium, sentiment analysis, translation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">project0201</t>
+  </si>
+  <si>
+    <t xml:space="preserve">project0202</t>
+  </si>
+  <si>
+    <t xml:space="preserve">project0203</t>
+  </si>
+  <si>
+    <t xml:space="preserve">project0204</t>
+  </si>
+  <si>
+    <t xml:space="preserve">¿De qué hablan las canciones? ¿Qué sentimiento expresan sus letras? ¿Y qué pasa con los géneros o los artistas? Este proyecto trata de arrojar un poco de luz sobre estas y otras preguntas.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Este el proyecto que he creado para mi tarea the mitad de Bootcamp en [IronHack](http://www.ironhack.com).  
+Tenía algunos requerimientos y restricciones como las siguientes:  
+1. Recolectar los datos por mi mismo (no se podían descargar conjuntos de datos)  
+2. El conjunto de datos recopilado debería de tener entre 30 and 100 observaciones (filas) y de 5 a 10 características (columnas)  
+3. Podría enriquecer el conjunto de datos con más información obtenida con otros métodos además del tecleo manual (por ejemplo, web scraping)  
+4. Necesidad de completar un análisis para responder las preguntas que tenía que resolver con este proyecto. También debería complementar el análisis con algún tipo de hipótesis.  
+##### Mi proyecto  
+Mis preguntas eran sobre las leras de las canciones que solemos escuchar cada día, estas preguntas son:  
+1. ¿Las letras de las canciones tienen un sentimiento positivo en general?  
+2. ¿Son las letras de las mujeres más positivas que las de los hombres?  
+3. ¿Son las letras de las canciones pop más positivas que las de hip hop?  
+&lt;img&gt;image1&lt;/img&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">##### Mi solución
+###### Python  
+- Creación del conjunto de datos usando python:  
+Decidí recopilar la información desde [Spotify Charts](https://charts.spotify.com/) porque quería analizar letras de canciones globales, así que escogí el top de artistas de la semana 47 del año 2022. El proceso que seguí fue teclear en un fichero los artistas de esa lista y además también usé [Last.fm](https://www.last.fm/) para recopilar y teclear más información como género, género musical general y si era una banda o grupo.  
+Entonces completé el conjunto de datos buscando las 10 canciones más populares de cada artista en [Spotify](https://open.spotify.com/) usando su API.  
+Después usé la librería de [__lyricsgenius__](https://pypi.org/project/lyricsgenius/) para conectar al sitio web de [Genius](https://genius.com/) para descargar 5 de las 10 canciones recopiladas in Spotify of every artist (porque el nombre de las canciones en Spotify no siempre tenía correspondencia en el nombre dado en Genius).  
+En este momento también creé una función con [Selenium](https://www.selenium.dev/) para obtener el token de conexión, por si acaso el tocken the conexión a Genius cambiaba.  
+Ahora mismo está almacenado en un fichero (secrets.txt) pero podría obtenerlo sin almacenarlo.
+&lt;img&gt;image2&lt;/img&gt; 
+- Análisis de sentimiento:  
+Una vez que descargué toda la información, necesité tratarla para realizar el análisis de sentimiento (using the library [__Flair__](https://github.com/flairNLP/flair)) y procesamiento de lenguaje natural ([__NLTK__](https://www.nltk.org/)).
+- Traducciones:  
+Puesto que la lista de canciones estaban cantadas en diferentes lenguajes, decidí traducir todo a inglés para simplificar el análisis. Para realizar esto usé la librería [__Fasttext__](https://fasttext.cc/) con su modelo pre-entrenado para detectar el idioma de las letras y entonces traducirlas a inglés con la librería [__translators__](https://github.com/uliontse/translators) la cual si no puede hacer la traducción, usa el traductor de Google para realizar el trabajo.
+- Top palabras:  
+Calculé el top de palabras con las funciones de NLTK y actualicé manualmente las palabras prohibidas de la lista para incluir más de las que no me interesaban en mi análisis.
+- Nube de palabras:  
+También creé una función para generar una nube de palabras con las librerías __wordcloud__ y __PIL__ para mostrar diferentes silueta que he descargado.
+- Análisis de hipótesis:  
+En otro documento de Jupyter, desarrolé el análisis de hipótesis y preparé el conjunto de datos para el análisis visual con [Tableau](https://public.tableau.com/)
+###### Tableau  
+Usé la versión públicva de Tableau para crear la presentación del proyecto y el análisis visual, lo puedes encontrar en [_mi Tableau_](https://public.tableau.com/app/profile/.scar.iglesias.roqueiro/viz/Mid-BootcampProject_16711135428210/Lyrics)  
+&lt;img&gt;image3&lt;/img&gt;
+###### Flask  
+El proyecto incluye una demo en Flask que permite la búsqueda de una canción de un artista y mostrará la letra con el top de palabras traducidas, el análisis de sentimiento y una nube de palabras.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Para resumir los enlaces de mi proyecto, aquí están:  
+- Video de presentación: [__Mi Youtube__](https://youtu.be/Veu5M7_hCUg)  
+- Visualizaciones: [__Mi Tableau__](https://public.tableau.com/app/profile/.scar.iglesias.roqueiro/viz/Mid-BootcampProject_16711135428210/Lyrics)  
+- Código fuente (incluida la demo en Flask): [__Mi Github__](https://github.com/oiroqueiro/mid-bootcamp-project)  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">tableau, visualización, dashboard, python, flask, web scrapping, API, Selenium, análisis de sentimiento, traducción, repository</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IHRepo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intelligent Helper Repository is my attempt to show how artificial intelligence can help in access to education.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is the project that I created for my Final Bootcamp project in Data Analytics in [IronHack](http://www.ironhack.com). The idea was to try to improve the Bootcamp experience, acquiring more students and helping the existing students. So I decided to transcribe all the videos of my boot camp, translate all the texts (to Spanish at least but some to Portuguese, Italian, German, Chinese, and Hindi, as the languages that could speak my fantastic cohort), caption them, creating a summary and keywords, all automatic (at this moment, couldn't finish all the automatism but exists all the functions for that).     
+&lt;img&gt;image1&lt;/img&gt;    
+The project also includes one app to search and find videos about one topic (or any word you want to use in any language that was translated) and when decide on the video you want to explore have the option to search inside the video and locate the exact moment where the video talk about your searching (Future feature, continue the implementing of the FULL TEXT index in MySQL with the option of Natural Language).   
+To play the videos with subtitles and locate in the exact position I used [VLC media player](https://www.videolan.org/vlc/index.es.html).   
+I would wanted to train my models but my hardware and the time made me change my mind, however, this project is not closed so maybe in the future I return here to improve it.    
+&lt;img&gt;image2&lt;/img&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">##### Process    
+- **Transcription**   
+For this task, I decided to use [Whisper](https://github.com/openai/whisper). After testing different options, this was which fitted more to my project. I used the model "base.en" because of my schedule (I had to create the project after work) and hardware requirements but can use others larger to get better performance, or even multi-language.   
+- **Subtitles**   I had many problems managing the subtitles, I tried to split the videos but synchronizing again the subtitles was impossible with the time I had to do it, so in the end I decided to use [Stable Whisper](https://github.com/jianfch/stable-ts) without split the video.   
+- **Summary**   For this task, I decided to use [Hugging Face transformers](https://huggingface.co/docs/transformers/index) after trying other options, I also tried many different models and decided to use [**mrm8488/flan-t5-large-finetuned-openai-summarize_from_feedback**](https://huggingface.co/mrm8488/flan-t5-large-finetuned-gsm8k) which gave me better results.   
+- **Keywords**   [**KeyBERT**](https://maartengr.github.io/KeyBERT/) was the chosen between some alternatives and the model I used was [**universal-sentence-encoder**](https://tfhub.dev/google/universal-sentence-encoder/4)   
+- **Translation**   This was the only part that didn't try other options because I used it before and worked fine for me but this also was not a smooth path, &lt;u&gt; Beware that translating subtitles can give you some surprises (break lines...)&lt;/u&gt; so I decided to split the subtitles into lines and translate them to joined together at the end.   
+- **BBDD**   
+This process stores in one [__MySQL__](https://www.mysql.com/) database all the texts I got (originals and translations) with the relationship with the videos. I created a FULL-TEXT index in the database so I could use the natural language option to search the videos.   
+- **APP**   Since I tried Flask in my [__Lyrics__](https://github.com/oiroqueiro/mid-bootcamp-project) project, for this project I wanted to try other options and after researching Streamlit and Django, I decided to take the complicated path, so I used [__Django__](https://www.djangoproject.com/) (with [__Bootstrap 5__](https://getbootstrap.com/)).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;img&gt;image3&lt;/img&gt;
+As I said before, the limited time didn't allowed me to finish everything I had in my mind (launch all the logic from Django, update videos, option to transcribe online videos (at the moment only can use files).  But I think in this project there are a lot of information about this complicated path I had chosen.
+To summarize the links of my project, here they are:  
+- Presentation video: [__My Youtube__](https://youtu.be/mbKBJYidxc4)  
+- Hackshow video: [__My Youtube__](https://youtu.be/Veu5M7_hCUg)  
+- Source codes (including the Django App): [__My Github__](https://github.com/oiroqueiro/final-project-bootcamp)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python, django, mysql, bbdd, trasnscription, subtitles, summary, keywords, translation, repository, video</t>
+  </si>
+  <si>
+    <t xml:space="preserve">project0301</t>
+  </si>
+  <si>
+    <t xml:space="preserve">project0302</t>
+  </si>
+  <si>
+    <t xml:space="preserve">project0303</t>
+  </si>
+  <si>
+    <t xml:space="preserve">project0304</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intelligent Helper Repository (Ayudante Inteligente de Respositorio) es mi intento por mostrar como la inteligencia artificial puede ayudar en el acceso a la educación.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Este es el proyecto que creé para mi tarea de final de Bootcamp en el curso de Análisis de Datos en [IronHack](http://www.ironhack.com). La idea era intentar mejorar la experiencia del Bootcamp, adquiriendo más estudiantes y ayudando a los existentes. Así que decidí transcribir todos los videos de mi bootcamp, traduciendo todos los textos (a español por lo menos pero alguno también a portugué, italiano, alemán, chino e hindi, como los idiomas que mi fantásticos compañeros y profesores podían hablar), suntitulando, creando resúmenes del contenido y palabras clave, todo automatizado (en este momento, no pude terminar todos los automatismos pero existen todas las funciones para ello).  
+&lt;img&gt;image1&lt;/img&gt;
+El proyecto también incluye una aplicación para buscar y encontrar videos que hablen sobre un tema (o cualquier palabra que se quiera buscar en cualquiera de los idiomas en que están traducidos los videos) y cuando se encuentra el video que se desea explorar, da la opción de hacer una búsqueda dentro del video y localizar el momento exacto donde se habla sobre lo que se está buscando (futura característica, continuar implementando los índices FULL TEXT en MySQL con la opción de Lenguaje Natural).  
+Para reproducir los videos con subtitulos y localizar la posición exacta he usado [VLC media player](https://www.videolan.org/vlc/index.es.html).  
+Me gustaría poder entrenar mis propios modelos pero el hardware de mi pc y el tiempo me hicieron desistir, sin embargo el proyecto no está cerrado y quizás en un futuro puedo volver a él para mejorarlo.
+&lt;img&gt;image2&lt;/img&gt;</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">##### Proceso   
+- **Transcripción**  
+Para esta tarea decidí usar [Whisper](https://github.com/openai/whisper). Después de probar diferentes opciones, esta fue la que se ajustaba mejor a mi proyecto. Usé el modelo "base.en" debido a mi calendario (tengo un trabajo a tiempo completo, con lo que el proyecto tenía que desarrollarlo después de mi trabajo) y los requerimientos de hardwaree requirements pero se puede usar otro modelo más pesado para obtener mejor resultado, o incluso multi-idioma.  
+- **Subtítulos**  
+Tuve muchos problemas para gestionar los subtítulos, Intenté partir los videos pero el sincronizarlos de nuevo se volvió imposible con el tiempo que tenía para hacerlo, así que al final decidí usar [Stable Whisper](https://github.com/jianfch/stable-ts) sin partir los videos.  
+- **Resumir**  
+Para esta tarea decidí usar [Hugging Face transformers](https://huggingface.co/docs/transformers/index) después de probar otras opciones, también probé varios modelos distintos y al final decidí usar [**mrm8488/flan-t5-large-finetuned-openai-summarize_from_feedback**](https://huggingface.co/mrm8488/flan-t5-large-finetuned-gsm8k) el cual me dio los mejores resultados.  
+- **Palabras clave**  
+[**KeyBERT**](https://maartengr.github.io/KeyBERT/) fue la opción escogida entre varias alternativas y el the model que usé fue [**universal-sentence-encoder**](https://tfhub.dev/google/universal-sentence-encoder/4)  
+- **Traducción**  
+Esta fue la única parte en la que no probé alternativas porque lo había utilizado anteriormente en mi proyecto Lyrics y funcionó perfectamente para mi aunque no fue un camino de rosas, &lt;u&gt;cuidado al traducir subtítulos ya que te pueden dar algunas sorpresas (saltos de líneas...)&lt;/u&gt; así que decidí partir los subtítulos en líneas, traducirlas y unirlas luego todas juntas al final.  
+- **Base de datos**  
+En este proceso guardé en una base de datos [__MySQL__](https://www.mysql.com/) todos los textos que tenía (originales y traducciones) con su relación con los videos. Creé un índice FULL TEXT en la base de datos por lo que pude usar la opción de búsqueda con lenguaje natural para buscar los videos.  
+- **Aplicación**  
+Ya que usé Flask en mi proyecto [__Lyrics__](https://github.com/oiroqueiro/mid-bootcamp-project) project, para este proyecto quería intentar alguna otra opción y después de investigar sobre Streamlit y Django, decidí tomar el camino más complicado, así que usé [__Django__](https://www.djangoproject.com/) (con [__Bootstrap 5__](</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">https://getbootstrap.com</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">/)).</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;img&gt;image3&lt;/img&gt;
+Como dije anteriormente, el límite de tiempo no me permitó terminar todo lo que tenía en mi cabeza (lanzar la lógica desde Django, actualizar videos, opción de transcribir videos online -de momento solo pude usar ficheros en local-).  Pero pienso que en este proyecto hay un montón de información sobre esta complicada travesía que escogí.
+Para resumir los enlaces de mi proyecto, aquí están:  
+- Video de presentación: [__My Youtube__](https://youtu.be/mbKBJYidxc4)  
+- Video en el Hackshow: [__My Youtube__](https://youtu.be/Veu5M7_hCUg)  
+- Código fuente (incluida la aplicación de Django): [__My Github__](https://github.com/oiroqueiro/final-project-bootcamp)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python, django, mysql, base de datos, transcripción, subtítulos, resumen, palabras clave, traducción, repositorio, video</t>
   </si>
   <si>
     <t xml:space="preserve">Portfolio</t>
   </si>
   <si>
-    <t xml:space="preserve">Personal portfolio from scratch to show my projects</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Long time I was thinking on configure one portfolio to show my projects but using one website with predefined templates threw me off.
-So I decided to create one portfolio from scratch and use the time I dedicate to it wisely to **improve my skills** and **learn more technologies** that could be *useful* in the future.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#### TEST
-- One
-- Two
-&lt;h6&gt;How I could do it if I am not an websites developer neither UX designer?&lt;/h6&gt;&lt;br&gt;&lt;br&gt;
-The solution came to me one day when I discovered [**Hugo**](https://gohugo.io/), a framework to building websites using templates, one of the best part is that there are a lot of them and many are free to use, so with my aknowledge of **Python** and **Flask** I decided to go for it. &lt;br&gt;
-During the time I was developing this project I faced many challenges and problems, mainly because what I wanted for my personal portfolio was some features that I thought that were mandatory:&lt;br&gt; &lt;li&gt;Responsive&lt;/li&gt; &lt;li&gt;Dark/Light mode&lt;/li&gt; &lt;li&gt;Multilanguage&lt;/li&gt; &lt;li&gt;Easy to use&lt;/li&gt; &lt;li&gt;Customizable&lt;/li&gt; &lt;li&gt;and I needed to like the template.&lt;/li&gt;&lt;br&gt; 
-So to get this I had find a beautiful template (to my liking), understand it, transform it to dynamic Flask templates and develope all the logic around them.  To store the information I wanted to use a new database that I had never use, then I was researching and decided to use [**SQLite**](https://www.sqlite.org/index.html) also free of charge and for this kind of projects very fast. At the beginning I thought to develope one solution inside the portfolio to mantain the data but I focused in made it usable as soon as possible so maybe this will be a future feature, neverthless I prepared all the authentication requirements (users, login, logout, menu) to reuse later. For this I developed a feature that make me feel a little proud of it which is **customized urls for the login and logout** so it would be more complicated for *bad people* to know that there is a door to enter in the website. When I realized that mantain the data inside the website would take time that I should to dedicate to other tasks, I decided to create a feature to insert all the data (languages, texts of the porftolio, personal data, projects) *using an excel template* which is easy to create and to insert.&lt;br&gt;&lt;br&gt;
-Regarding to the multilanguage function, I could use some libraries like [*Babel*](https://babel.pocoo.org/en/latest/) like I saw in many websites but I think that the purpose of a portfolio is to show the knowledge that the owner has so need to translate all the texts by the own user, that’s why I included in the template one section to enter the languages and columns in the other sections. I mean, if anyone prefer to have the portfolio translated to the most possible languages, it’s ok, but I think that if the purpose of the portfolio is to communicate with others, it’s better to show the options that can use for it.&lt;br&gt;&lt;br&gt;
-And almost at the end of the building of my portfolio, and before start with the technologies that I had in my mind to try ( [**Elasticsearch**](https://www.elastic.co/elasticsearch/) y [**Docker**](https://www.docker.com/) ), the way I thought that could be useful to customize a little bit more the content was the use of [**Markdown**](https://www.markdownguide.org/), so at the end this become another feature of my portfolio.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;img&gt;image1&lt;/img&gt;
-And this is my project, you are using a *live demo* right now because this is the result of  **all the hours I’ve dedicated** to this project. If you want to read more, you can go to [my repository in Github](https://github.com/oiroqueiro) and see the source code.
-&lt;img&gt;image2&lt;/img&gt; 
- and the final image: 
- &lt;img&gt;image3&lt;/img&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Python, Flask, SQLite, Docker, Elastic Search, Creative Problem Solving</t>
-  </si>
-  <si>
-    <t xml:space="preserve">portfolio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Portfolio personal desde cero para mostrar mis proyectos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Durante bastante tiempo estuve pensando en configurar un portfolio para mostrar mis proyectos pero user una página web con plantillas predefinidas me echaba para atrás.
-Así que decidí crear un portfolio desde cero y aprovechar bien el tiempo dedicado a ello para **mejorar mis habilidades** y **aprender más tecnologías** que podrían ser *útiles* en el futuro.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;h6&gt;¿Cómo podría hacerlo si no soy desarrollador de sitios web ni diseñador de UX?&lt;/h6&gt;
-&lt;br&gt;&lt;br&gt;La solución me llegó un día cuando descubrí [**Hugo**](https://gohugo.io/), un *framework* para crear sitios web usando plantillas, una de las mejores partes es que hay muchas y de ellas bastantes son de uso gratuito, así que con mi conocimiento de **Python** y **Flask** decidí hacerlo.&lt;br&gt;
-Durante el tiempo que estuve desarrollando este proyecto me enfrenté a muchos desafíos y problemas, principalmente porque lo que quería para mi portafolio personal eran algunas características que pensaba que eran obligatorias:&lt;br&gt;
- - Responsivo  - Modo oscuro/claro - Multi lenguaje - Fácil de usar - Personalizable - y necesitaba que me gustara la plantilla&lt;br&gt;
-Entonces, para lograr esto, encontré una hermosa plantilla (para mi gusto), la entendí, la transformé en plantillas dinámicas de Flask y desarrollé toda la lógica que las rodea.  Para almacenar la información quería usar una nueva base de datos que nunca había usado, entonces estuve investigando y decidí usar [**SQLite**](https://www.sqlite.org/index.html) también gratuita y para este tipo de proyectos muy rápido. Al principio pensé en desarrollar una solución dentro del portfolio para mantener los datos, pero me concentré en hacerla utilizable lo antes posible, por lo que tal vez esto sea una característica futura, sin embargo, preparé todos los requisitos de autenticación (usuarios, inicio de sesión, cierre de sesión, menú) para reutilizar más tarde. Para esto desarrollé una característica que me hace sentir un poco orgulloso de ella que es **URL personalizadas para iniciar y cerrar sesión** por lo que sería más complicado para la *gente mala* saber que hay una puerta para entrar en el sitio web. Cuando me di cuenta de que mantener los datos dentro del sitio web tomaría tiempo que debería dedicar a otras tareas, decidí crear una funcionalidad para insertar todos los datos (idiomas, textos del portafolio, datos personales, proyectos) *usando una plantilla de excel* que es fácil de crear e insertar.&lt;br&gt;&lt;br&gt;
-En cuanto a la función multilenguaje, podría usar algunas bibliotecas como [*Babel*](https://babel.pocoo.org/en/latest/) como vi en muchos sitios web pero creo que el propósito de un portfolio es mostrar el conocimiento que tiene el propietario por lo que necesita traducir todos los textos por si mismo, por eso incluí en la plantilla una sección para ingresar los idiomas y columnas en las otras secciones. Quiero decir, si alguien prefiere traducir el portafolio a la mayor cantidad de idiomas posibles, está bien, pero creo que si el propósito del portfolio es comunicarse con otros, es mejor mostrar las opciones que pueden utilizar para ello.&lt;br&gt;&lt;br&gt;
-Y casi al final del desarrollo de mi portfolio, y antes de comenzar con las tecnologías que tenía en mente probar ([**Elastic Search**](https://www.elastic.co/elasticsearch/) y [**Docker**](https://www.docker.com/)), la manera que pensé que podría ser más útil para personalizar un poco más el contenido fue el uso de [**Markdown**](https://www.markdownguide.org/), así que al final esto se convirtió en otra característica de mi portfolio.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;img&gt;image1&lt;/img&gt; 
-Y este es mi proyecto, tú estás usando una *demo en vivo* porque este es el resultado de **todas las horas que le he dedicado** al proyecto. Si quieres leer más, puedes visitar [mi repositorio ie Github](https://github.com/oiroqueiro) y ver el código fuente. 
-&lt;img&gt;image2&lt;/img&gt;
-y la imagen final:   
- &lt;img&gt;image3&lt;/img&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Python, Flask, SQLite, Docker, Elastic Search, Resolución Creativa de Problemas</t>
+    <t xml:space="preserve">Portfolio built from scratch, from website planning with no idea of web development to deployment with docker without idea of containers.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I had several projects that I wanted to show but I didn't like the idea of using one existent website because all the alternatives that I was trying didn't have some of the features I thought were a must in my portfolio or were not flexible to customize it or were not beautiful (or what I consider beautiful for a portfolio).  
+Using one of those platforms would be the best option since I have a full-time job and two little girls born during the pandemic years, but I decided to go for it through the complicated path (sometimes hell path) and &lt;u&gt;create my portfolio from scratch&lt;/u&gt;.  
+I know that one portfolio is not a good example for a data analytics project, actually is not related to data analytics, but this project was a great opportunity to show my determination, creative problem solving, adaptability and to learn a lot along the time I would dedicate to this project.  
+The features I wanted in my portfolio include:  
+1. Multi-language 
+2. Responsive website 
+3. Light/Dark mode 
+4. Customizable 
+5. Containerized 
+6. Index Search  
+The first four were mandatory, the other two I wanted to learn and practice.  
+So let's explain the path from the beginning.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#### **The path**  
+Since I am not a UX/Designer or web developer, and my knowledge of HTML, CSS, and JavaScript was limited, the challenge started being super hard for me.   
+##### **The website**  When I started to investigate my options to create one website, the beginning was very discouraging. Only when I discovered [**Hugo**](https://gohugo.io/) I started to see the light at the end of the tunnel. Hugo is a framework for building websites with a lot of beautiful templates for websites and a great community. So I was researching Hugo and his templates for quite a while until I found some templates that could fit my requirements. The problem was that Hugo is fantastic for building static websites which is the opposite of my idea of one portfolio.  
+So in the end when I chose the [**iWriter**](https://github.com/statichunt/iwriter-hugo) template arrived at the moment to adapt it to a dynamic website.  
+##### **Flask**  One technology that I wanted to explore and improve my skills in was [**Python**](https://www.python.org/) because has tons of libraries, frameworks, and an impressive community behind it. So, when I thought about dynamic websites, [**Flask**](https://flask.palletsprojects.com/en/3.0.x/) came quickly to my mind. Since I worked with it in my [*Lyrics*](https://github.com/oiroqueiro/mid-bootcamp-project) project, I knew about his capabilities but the hard work had just started.  
+I had to adapt the iWriter template to be a dynamic template with [Jinja](https://jinja.palletsprojects.com/en/3.1.x/templates/) without losing any functionality I liked about this template.  
+After spending many, many, many hours understanding the HTML, CSS, javascript, and Bootstrap (and other technologies) that my template was used to have such features and more hours cleaning the code and adapting, I had some templates quite cleaned and ready to use with the logic of my website.  
+At this point I want to share with all of you [**this fantastic tutorial of Flask**](https://blog.miguelgrinberg.com/post/the-flask-mega-tutorial-part-i-hello-world), by *Miguel Grinberg*. I also use this one, in Spanish, of [**j2logo**](https://j2logo.com/tutorial-flask-espanol/) by *Juan José Lozano Gómez*. I learned a lot with them and with all the features that I had to face.  
+##### **Customizable**  I wanted a customizable website so after evaluating different options, I decided to use one Excel file to store all the texts of my website in addition to the content of my portfolio. The menus texts, buttons, images, ... can be adapted easily.  
+At the beginning I thought to manage the creation of the content within the website, but soon I realized that I didn't have time if I wanted to finish the project this year. Nevertheless, I did investigate and in the end, I could create one part that makes me feel a little proud of, it is that I could make the URLs to the login and logout pages of my website customizable via environment variables. The option of editing the content would be a future feature.  
+And how could I make the content of my portfolio customizable? Firstly I thought about the use of HTML, then the use of [**Markdown**](https://www.markdownguide.org/), and in the end, I thought what's better than allowing the use of both? So, we can write our content using Markdown and HTML labels and use both at the same time.  
+##### **DDBB**  
+I have been working with Microsoft SQL Server for more than 15 years and lately, I have been working with MySQL, at the beginning of my career I was using for years Oracle. So for this project, I decided to try a new one and the choice for developing was [**SQLite**](https://www.sqlite.org/index.html) but to use it in production once I deploy the project I went for [**PostgreSQL**](https://www.postgresql.org/). The good part is that the portfolio works perfectly with both so only changing the environment variables can use SQLite, PostgreSQL, or another different.  
+##### **The search**  
+In the beginning, my portfolio would have very few projects, so a searching function would not be too important but I wanted to create one project alive for a long time and easily maintainable so in the end I implemented a simple search function using the queries of the extension [**FlaskSQLAlchemy**](https://flask-sqlalchemy.palletsprojects.com/en/3.1.x/) which was the library that I was using to work with the databases. But in the last months I have been reading quite often about NoSQL databases, and the capabilities of [**Elasticsearch**](https://www.elastic.co/) for searching, so I decided to start working with this kind of databases using Elasticsearch in my project.  
+Finally, the option of search in my portfolio is powered by Elasticsearch and, in case this engine is not present in our enviroment, will be powered by FlaskSQLAlchemy.  
+I also have a search of keywords, this is much simpler and it will find only the keyword we are searching but with the characteristic of bringing the keywords that share the projects where our keyword search is present too.  
+##### **Containerization**  
+And, if all the technologies I had to explore, learn, and implement for my project were not enough, I decided that I should containerize my app. So I started to learn **Docker** since this is one of the most popular platforms. During my learning path, I was able to create a docker container with my Flask app, so I had one docker container with my portfolio working but I wanted to create all my whole project with containers. In the end, I finished with a docker network with 3 containers:   
+- The first one, and more important because has all the data, one PostgreSQL docker 
+- The second one, if present, is the Elasticsearch docker for the searching functionality 
+- The third one is my Flask app which has even the HTTP Server powered by [**Gunicorn**](https://gunicorn.org/)  
+##### **Deployment**  
+(I am still working on this part)  
+As the last step of my project, I need to deploy it. During this path, I was working always with opensource or free-of-charge options (except the domain name that I had to pay) and the option I found that could work for me was the use of [**OCI**](https://www.oracle.com/es/cloud/), the **Oracle Cloud Infrastructure** that has one Free Tier (Always Free Services) which I could use for the deployment.  
+In addition to this, I created one [**Google Analytics**](https://analytics.google.com/) account to monitor and analyze my website.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">To summarize, the links of this project are:
+- All the source code (including the docker and compose files): [**My Github**](https://github.com/oiroqueiro/portfolio)
+- Live demo: [**my Portfolio Website**](</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">http://www.oscarlytics.com</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -903,7 +1016,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -964,6 +1077,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2381,12 +2498,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:X25"/>
+  <dimension ref="A1:X9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2398,7 +2515,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="43.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="19.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="17.7"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="24" min="9" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="68.05"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="24" min="10" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2463,7 +2581,7 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="650.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="13" t="n">
         <v>44890</v>
       </c>
@@ -2501,7 +2619,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="13" t="n">
         <v>44890</v>
       </c>
@@ -2539,9 +2657,9 @@
         <v>179</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="13" t="n">
-        <v>44986</v>
+        <v>44912</v>
       </c>
       <c r="B4" s="12" t="n">
         <v>1</v>
@@ -2555,13 +2673,13 @@
       <c r="E4" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="15" t="s">
         <v>190</v>
       </c>
       <c r="I4" s="1" t="s">
@@ -2571,12 +2689,18 @@
         <v>192</v>
       </c>
       <c r="P4" s="5" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>193</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="13" t="n">
-        <v>44986</v>
+        <v>44912</v>
       </c>
       <c r="B5" s="8" t="n">
         <v>1</v>
@@ -2588,30 +2712,36 @@
         <v>186</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="P5" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="Q5" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="R5" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="13" t="n">
-        <v>45017</v>
+        <v>44996</v>
       </c>
       <c r="B6" s="12" t="n">
         <v>1</v>
@@ -2620,34 +2750,40 @@
         <v>1</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>205</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="L6" s="5"/>
       <c r="O6" s="5" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="P6" s="5" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>208</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="13" t="n">
-        <v>45017</v>
+        <v>44996</v>
       </c>
       <c r="B7" s="12" t="n">
         <v>1</v>
@@ -2656,34 +2792,40 @@
         <v>2</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="G7" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="L7" s="5"/>
+      <c r="O7" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="P7" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="I7" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="L7" s="5"/>
-      <c r="O7" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Q7" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="292.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="13" t="n">
-        <v>45047</v>
+        <v>45287</v>
       </c>
       <c r="B8" s="12" t="n">
         <v>1</v>
@@ -2692,33 +2834,24 @@
         <v>1</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>209</v>
+        <v>216</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="O8" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="P8" s="5" t="s">
-        <v>215</v>
+        <v>217</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="13" t="n">
-        <v>45047</v>
+        <v>45287</v>
       </c>
       <c r="B9" s="12" t="n">
         <v>1</v>
@@ -2729,190 +2862,17 @@
       <c r="D9" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="O9" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="13" t="n">
-        <v>45078</v>
-      </c>
-      <c r="B10" s="12" t="n">
-        <v>1</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="O10" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="P10" s="5" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="13" t="n">
-        <v>45078</v>
-      </c>
-      <c r="B11" s="12" t="n">
-        <v>1</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="O11" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="P11" s="5" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="11.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="13" t="n">
-        <v>45170</v>
-      </c>
-      <c r="B12" s="12" t="n">
-        <v>1</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>234</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>235</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>236</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="O12" s="5" t="s">
-        <v>238</v>
-      </c>
-      <c r="P12" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="Q12" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="R12" s="1" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="13" t="n">
-        <v>45170</v>
-      </c>
-      <c r="B13" s="12" t="n">
-        <v>1</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="O13" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="P13" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="Q13" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="R13" s="1" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I14" s="5"/>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L25" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H2" r:id="rId1" display="So, if you want to see the result of this project, you can go to [**One story about Life Expectancy**](https://public.tableau.com/views/TableauProject_16693794082020/Presentation?:language=en-US&amp;:display_count=n&amp;:origin=viz_share_link)"/>
     <hyperlink ref="H3" r:id="rId2" display="Así que, si quieres ver el resultado de este proyecto, puedes ir a [**Una historia sobre Esperanza de Vida**](https://public.tableau.com/views/TableauProject_16693794082020/Presentation?:language=en-US&amp;:display_count=n&amp;:origin=viz_share_link)"/>
+    <hyperlink ref="H4" r:id="rId3" display="To summarize the links of my project, here they are:  &#10;&#10;- Presentation video: [__My Youtube__](https://youtu.be/Veu5M7_hCUg)  &#10;- Visualizations: [__My Tableau__](https://public.tableau.com/app/profile/.scar.iglesias.roqueiro/viz/Mid-BootcampProject_16711135428210/Lyrics)  &#10;- Source codes (including the Flask App): [__My Github__](https://github.com/oiroqueiro/mid-bootcamp-project)&#10;"/>
+    <hyperlink ref="G5" r:id="rId4" display="##### Mi solución&#10;  &#10;###### Python  &#10;  &#10;- Creación del conjunto de datos usando python:  &#10;Decidí recopilar la información desde [Spotify Charts](https://charts.spotify.com/) porque quería analizar letras de canciones globales, así que escogí el top de artistas de la semana 47 del año 2022. El proceso que seguí fue teclear en un fichero los artistas de esa lista y además también usé [Last.fm](https://www.last.fm/) para recopilar y teclear más información como género, género musical general y si era una banda o grupo.  &#10;Entonces completé el conjunto de datos buscando las 10 canciones más populares de cada artista en [Spotify](https://open.spotify.com/) usando su API.  &#10;Después usé la librería de [__lyricsgenius__](https://pypi.org/project/lyricsgenius/) para conectar al sitio web de [Genius](https://genius.com/) para descargar 5 de las 10 canciones recopiladas in Spotify of every artist (porque el nombre de las canciones en Spotify no siempre tenía correspondencia en el nombre dado en Genius).  &#10;En este momento también creé una función con [Selenium](https://www.selenium.dev/) para obtener el token de conexión, por si acaso el tocken the conexión a Genius cambiaba.  &#10;Ahora mismo está almacenado en un fichero (secrets.txt) pero podría obtenerlo sin almacenarlo.&#10;&lt;img&gt;image2&lt;/img&gt; &#10;- Análisis de sentimiento:  &#10;Una vez que descargué toda la información, necesité tratarla para realizar el análisis de sentimiento (using the library [__Flair__](https://github.com/flairNLP/flair)) y procesamiento de lenguaje natural ([__NLTK__](https://www.nltk.org/)).&#10;- Traducciones:  &#10;Puesto que la lista de canciones estaban cantadas en diferentes lenguajes, decidí traducir todo a inglés para simplificar el análisis. Para realizar esto usé la librería [__Fasttext__](https://fasttext.cc/) con su modelo pre-entrenado para detectar el idioma de las letras y entonces traducirlas a inglés con la librería [__translators__](https://github.com/uliontse/translators) la cual si no puede hacer la traducción, usa el traductor de Google para realizar el trabajo.&#10;- Top palabras:  &#10;Calculé el top de palabras con las funciones de NLTK y actualicé manualmente las palabras prohibidas de la lista para incluir más de las que no me interesaban en mi análisis.&#10;- Nube de palabras:  &#10;También creé una función para generar una nube de palabras con las librerías __wordcloud__ y __PIL__ para mostrar diferentes silueta que he descargado.&#10;- Análisis de hipótesis:  &#10;En otro documento de Jupyter, desarrolé el análisis de hipótesis y preparé el conjunto de datos para el análisis visual con [Tableau](https://public.tableau.com/)&#10;&#10;###### Tableau  &#10;Usé la versión públicva de Tableau para crear la presentación del proyecto y el análisis visual, lo puedes encontrar en [_mi Tableau_](https://public.tableau.com/app/profile/.scar.iglesias.roqueiro/viz/Mid-BootcampProject_16711135428210/Lyrics)  &#10;&#10;&lt;img&gt;image3&lt;/img&gt;&#10;&#10;###### Flask  &#10;El proyecto incluye una demo en Flask que permite la búsqueda de una canción de un artista y mostrará la letra con el top de palabras traducidas, el análisis de sentimiento y una nube de palabras."/>
+    <hyperlink ref="H5" r:id="rId5" display="Para resumir los enlaces de mi proyecto, aquí están:  &#10;&#10;- Video de presentación: [__Mi Youtube__](https://youtu.be/Veu5M7_hCUg)  &#10;- Visualizaciones: [__Mi Tableau__](https://public.tableau.com/app/profile/.scar.iglesias.roqueiro/viz/Mid-BootcampProject_16711135428210/Lyrics)  &#10;- Código fuente (incluida la demo en Flask): [__Mi Github__](https://github.com/oiroqueiro/mid-bootcamp-project)  "/>
+    <hyperlink ref="H6" r:id="rId6" display="&lt;img&gt;image3&lt;/img&gt;&#10;&#10;As I said before, the limited time didn't allowed me to finish everything I had in my mind (launch all the logic from Django, update videos, option to transcribe online videos (at the moment only can use files).  But I think in this project there are a lot of information about this complicated path I had chosen.&#10;&#10;To summarize the links of my project, here they are:  &#10;- Presentation video: [__My Youtube__](https://youtu.be/mbKBJYidxc4)  &#10;- Hackshow video: [__My Youtube__](https://youtu.be/Veu5M7_hCUg)  &#10;- Source codes (including the Django App): [__My Github__](https://github.com/oiroqueiro/final-project-bootcamp)"/>
+    <hyperlink ref="G7" r:id="rId7" display="https://getbootstrap.com"/>
+    <hyperlink ref="H8" r:id="rId8" display="http://www.oscarlytics.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
preparing for the deployment
</commit_message>
<xml_diff>
--- a/content.xlsx
+++ b/content.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="147">
   <si>
     <t xml:space="preserve">language</t>
   </si>
@@ -304,60 +304,30 @@
     <t xml:space="preserve">name</t>
   </si>
   <si>
-    <t xml:space="preserve">Oscar Iglesias</t>
-  </si>
-  <si>
     <t xml:space="preserve">subtitle</t>
   </si>
   <si>
-    <t xml:space="preserve">Data Analyst &amp; ERP Developer Analyst. Welcome to my Portfolio.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Hola, soy</t>
   </si>
   <si>
-    <t xml:space="preserve">Analista de Datos &amp; Analista Desarrollador de ERP. Bienvenid@ a mi Portfolio.</t>
-  </si>
-  <si>
     <t xml:space="preserve">about</t>
   </si>
   <si>
-    <t xml:space="preserve">Hi,I’m Oscar Iglesias, Data Analyst and ERP Analyst Developer</t>
-  </si>
-  <si>
     <t xml:space="preserve">parragraph1</t>
   </si>
   <si>
-    <t xml:space="preserve">I'm living in Ourense, a small city of Spain with my wife and 2 little girls.</t>
-  </si>
-  <si>
     <t xml:space="preserve">parragraph2</t>
   </si>
   <si>
-    <t xml:space="preserve">I love working with data. During my professional experience, I got the chance to work with many types of databases and acquire a great experience helping stakeholders to get more information and discover good insights because of my skills in visualisation as well.</t>
-  </si>
-  <si>
     <t xml:space="preserve">parragraph3</t>
   </si>
   <si>
-    <t xml:space="preserve">Then, when my youngest baby was ready to be born I had the chance to join [**Ironhack**](https://www.ironhack.com/es/en/data-analytics/remote) to improve my skills of data mining and learn much more about analysis and artificial intelligence. 
-During this time I had to face many challenges that the teaching team provided us which I could solve, making me feel more confident with my skills and learning and creating projects (like my final project, Ironhack repository) that could help others to improve their skills too.
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">parragraph4</t>
   </si>
   <si>
-    <t xml:space="preserve">I consider myself a **team player** with great **adaptability** and **autonomy** as I had to learn almost by myself and start to create features for different ERP along the years. 
-My work colleagues would say I am a *hard-working* person that doesn’t hesitate to **help** others when they need to deliver an urgent job so they can reach on time.</t>
-  </si>
-  <si>
     <t xml:space="preserve">parragraph5</t>
   </si>
   <si>
-    <t xml:space="preserve">During my career I helped companies to manage their ERPs and Data so their employees, my colleagues, could dedicate more time to other tasks and be more productive.</t>
-  </si>
-  <si>
     <t xml:space="preserve">parragraph6</t>
   </si>
   <si>
@@ -370,58 +340,18 @@
     <t xml:space="preserve">skill1</t>
   </si>
   <si>
-    <t xml:space="preserve">Creative Problem Solving.</t>
-  </si>
-  <si>
     <t xml:space="preserve">skill2</t>
   </si>
   <si>
-    <t xml:space="preserve">Responsible.</t>
-  </si>
-  <si>
     <t xml:space="preserve">skill3</t>
   </si>
   <si>
-    <t xml:space="preserve">Adaptability.</t>
-  </si>
-  <si>
     <t xml:space="preserve">youtube</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.youtube.com/embed/8CAoLz4NS5o</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hola, soy Oscar Iglesias, Analista de Datos y Analista Desarrollador de ERP.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Estoy viviendo Ourense, una pequeña ciudad de España con mi mujer y mis dos niñas.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Me encanta trabajar con datos. Durante toda mi carrera profesional, tuve la oportunidad de trabajar con muchos tipos de bases de datos y adquirir una gran experiencia ayudando a las partes interesadas a obtener más información y descrubrir claves esclarecedoras debido, también, a mis habilidades en visualización de datos.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Entonces, cuando mi hija más pequeña estaba preparada para nacer, tuve la oportunidad de unirme al bootcamp de análisis de datos de [**Ironhack**](https://www.ironhack.com/es/en/data-analytics/remote) para mejorar mis habilidades de minería de datos y aprender mucho más de análisis e inteligencia artificial. 
-Durante este tiempo tuve que superar muchos retos que el equipo de enseñanza nos propuso, haciéndome sentir más confianza en mis habilidades y aprendiendo y creando proyectos (como mi proyecto final, Ironhack repository) que podrían ayudar a otros también a incrementar sus habilidades.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Me considero a mi mismo un **buen compañero de trabajo** con gran **adaptabilidad** y **autonomía** ya que he tenido que aprender por mi mismo a crear nuevas funcionalidades en los diferentes ERP a lo largo de los años. Mis compañeros de trabajo dirían que soy una *persona trabajadora* que no duda en **ayudar** a otros cuando lo necesitan.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Durante mi carrera he ayudado a muchas empresas a manejar su ERP y datos de manera que sus empleados, y en muchos casos mis compañeros, podían dedicar más tiempo a otras tareas y ser más productivos.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Mis habilidades</t>
   </si>
   <si>
-    <t xml:space="preserve">Resolución creativa de problemas.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Responsable.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adaptabilidad.</t>
-  </si>
-  <si>
     <t xml:space="preserve">contact</t>
   </si>
   <si>
@@ -467,9 +397,6 @@
     <t xml:space="preserve">email_subject</t>
   </si>
   <si>
-    <t xml:space="preserve">New message from Oscarlytics portfolio</t>
-  </si>
-  <si>
     <t xml:space="preserve">Vamos a conectar</t>
   </si>
   <si>
@@ -491,9 +418,6 @@
     <t xml:space="preserve">Enviar mensaje</t>
   </si>
   <si>
-    <t xml:space="preserve">Nuevo mensaje desde el portfolio Oscarlytics</t>
-  </si>
-  <si>
     <t xml:space="preserve">date</t>
   </si>
   <si>
@@ -540,434 +464,6 @@
   </si>
   <si>
     <t xml:space="preserve">image3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">One story about Life Expectancy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">How has Life Expectancy evolved over the years in the world? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">I was asked to create one dashboard using [**Tableau**](https://www.tableau.com/) and collect the data wherever I wanted. So I decided to go for *one story about Life Expectancy* but try to look at the data from a different perspective than the usual GDP or any economic reasons.  
-&lt;img&gt;image1&lt;/img&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Firstly I researched the different sources that I could use to create my database, since I wanted to analyze Life Expectancy over many years it was not easy to find different databases with the required information. In the end, I decided to use [*The World Bank*](https://www.worldbank.org/en/home) databases so I spent quite an amount of time digging into those databases.   
-When I downloaded all the interesting databases for my project (not all were useful), I had to process them with **python** to normalize the data and prepare one only database to use in **Tableau**.   
-The path since I started to create the dashboard brought to the front how human nature could affect Life Expectancy, for instance, the &lt;u&gt;genocides&lt;/u&gt; or the &lt;u&gt;basic sanitation services&lt;/u&gt;.  
-I tried to show the information like a *story*, starting in the year 1960 and finishing in the year 2020, unfortunately, the information didn't include the *pandemic of Covid* but I think that could be a little bit interesting all I could show in my dashboard like the Life Expectancy changing or the deviation from the mean in the 2020 year.   
-&lt;img&gt;image2&lt;/img&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">So, if you want to see the result of this project, you can go to [**One story about Life Expectancy**](https://public.tableau.com/views/TableauProject_16693794082020/Presentation?:language=en-US&amp;:display_count=n&amp;:origin=viz_share_link)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tableau, visualization, dashboard, python</t>
-  </si>
-  <si>
-    <t xml:space="preserve">project0101</t>
-  </si>
-  <si>
-    <t xml:space="preserve">project0102</t>
-  </si>
-  <si>
-    <t xml:space="preserve">project0103</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Una historia sobre Esperanza de Vida</t>
-  </si>
-  <si>
-    <t xml:space="preserve">¿Cómo ha evolucionado la Esperanza de Vida a lo largo de los años en el mundo?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Me pidieron que creara una presentación usando [**Tableau**](https://www.tableau.com/) recopilando los datos donde quisiera. Así que decidí buscar *una historia sobre Esperanza de Vida* pero tratando de ver los datos desde una perspectiva diferente a la del PIB habitual o cualquier razón económica. 
-&lt;img&gt;image1&lt;/img&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Primero estuve investigando las diferentes fuentes que podía utilizar para crear mi base de datos, ya que quería analizar la Esperanza de Vida a lo largo de muchos años no era fácil encontrar diferentes bases de datos con la información requerida. Al final decidí utilizar las bases de datos de [*The World Bank*](https://www.worldbank.org/en/home) así que dediqué bastante tiempo a investigar más en profundidad dichas bases datos.  
-Cuando descargué todas las bases de datos que consideré interesantes para mi proyecto (no todas eran útiles), tuve que procesarlas con **python** para normalizar los datos y preparar una única base de datos para usarla en **Tableau**.  
-El camino desde que comencé a crear el tablero sacó a relucir cómo la naturaleza humana podría afectar a la Esperanza de Vida, por ejemplo los  &lt;u&gt;genocidios&lt;/u&gt; o los &lt;u&gt;servicios básicos de saneamiento&lt;/u&gt;.  
-Intenté mostrar la información como un *historia*, empezando en el año 1960 y terminando en el año 2020, lamentablemente la información no incluía la *pandemia del Covid*  pero creo que podría ser un poco interesante todo lo que pude mostrar en my tablero como el cambio en la Esperanza de Vida o la desviación de la media en el año 2020.  &lt;img&gt;image2&lt;/img&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Así que, si quieres ver el resultado de este proyecto, puedes ir a [**Una historia sobre Esperanza de Vida**](https://public.tableau.com/views/TableauProject_16693794082020/Presentation?:language=en-US&amp;:display_count=n&amp;:origin=viz_share_link)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tableau, visualización, dashboard, python</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lyrics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What do the songs talk about? What is the sentiment of their lyrics? And what about the genres or the artists? This project tries to shed some light on this and other questions.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This is the project that I created for my Mid-Bootcamp task in [IronHack](http://www.ironhack.com).     
-I had some requirements and restrictions like:     
-1. Collect the data by myself (cannot download datasets)  
-2. The dataset should have between 30 and 100 observations (rows) and 5 to 10 features (columns)  
-3. I could enrich the dataset with more information obtained with other methods than manual typing (for example, web scraping)  4. Need to complete one analysis to answer the questions that I have to solve with this project, also I should supplement the analysis with some hypothesis.     
-##### My project   
-My questions were about the lyrics of the songs that we use to listen every day, these questions are:     
-1. Do the lyrics have an overall positive sentiment?  
-2. Are women's lyrics more positive than men's  
-3. Are pop's lyrics better than hip hop's?     
-&lt;img&gt;image1&lt;/img&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">##### My solution     
-###### Python      
-- Creation of the dataset using Python:   
-I decided to collect information from [Spotify Charts](https://charts.spotify.com/) because I wanted to analyze lyrics globally, so I chose the top artist of week 47 of the year 2022. The process I followed was to type in a file the artist of that chart and also use [Last.fm](https://www.last.fm/) to type more information like gender, main genre and if is a band.  
-Then I complete the dataset by searching the 10 most popular songs of every artist in [Spotify](https://open.spotify.com/) using their API.   
-After that, I used the [__lyricsgenius__](https://pypi.org/project/lyricsgenius/) library to connect to the website [Genius](https://genius.com/) to download 5 lyrics of the 10 most popular songs in Spotify of every artist (because the name of the songs in Spotify not always has a corresponding name in Genius).   
-At this point, I also created one function with [Selenium](https://www.selenium.dev/) to get the connection token, just in case the token to connect to Genius changes.   
-Right now is stored in a file (secrets.txt) but could get it without storing it.   
-&lt;img&gt;image2&lt;/img&gt;  
-- Sentiment Analysis:   
-Once I downloaded all the information, needed to make a treatment to do the sentiment analysis (using the library [__Flair__](https://github.com/flairNLP/flair)) and natural language processing ([__NLTK__](https://www.nltk.org/)).  
-- Translations:   
-Since the list of songs was used in different languages, I decided to translate all into English to simplify the analysis. For this, I used the library [__Fasttext__](https://fasttext.cc/) with their pre-trained model to detect the language of the lyrics and then translate them to English with the library [__translators__](https://github.com/uliontse/translators) which if cannot do the translation uses google translator to perform the work.   
-- Top words:   
-I calculated the top words with NLTK functions and update manually their stop words list to include more that where not interesting to my analysis.  
-- Wordcloud:   
-I also created a function to generate a one-word cloud with the library __wordcloud__ and __PIL__ to show different shapes that I downloaded.  
-- Hypothesis analysis:   
-In another Jupyter notebook, I developed the hypothesis analysis and prepared the dataset for the visual analysis with [Tableau](https://public.tableau.com/)    
-###### Tableau   
-I used Tableau in his public version to create the presentation of the project and the visual analysis of the project, which can be found in [_my Tableau_](https://public.tableau.com/app/profile/.scar.iglesias.roqueiro/viz/Mid-BootcampProject_16711135428210/Lyrics)     
-&lt;img&gt;image3&lt;/img&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">To summarize the links of my project, here they are:  
-- Presentation video: [__My Youtube__](https://youtu.be/Veu5M7_hCUg)  
-- Visualizations: [__My Tableau__](https://public.tableau.com/app/profile/.scar.iglesias.roqueiro/viz/Mid-BootcampProject_16711135428210/Lyrics)  
-- Source codes (including the Flask App): [__My Github__](https://github.com/oiroqueiro/mid-bootcamp-project)
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tableau, visualization, dashboard, python, flask, web scrapping, API, Selenium, sentiment analysis, translation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">project0201</t>
-  </si>
-  <si>
-    <t xml:space="preserve">project0202</t>
-  </si>
-  <si>
-    <t xml:space="preserve">project0203</t>
-  </si>
-  <si>
-    <t xml:space="preserve">project0204</t>
-  </si>
-  <si>
-    <t xml:space="preserve">¿De qué hablan las canciones? ¿Qué sentimiento expresan sus letras? ¿Y qué pasa con los géneros o los artistas? Este proyecto trata de arrojar un poco de luz sobre estas y otras preguntas.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Este el proyecto que he creado para mi tarea the mitad de Bootcamp en [IronHack](http://www.ironhack.com).  
-Tenía algunos requerimientos y restricciones como las siguientes:  
-1. Recolectar los datos por mi mismo (no se podían descargar conjuntos de datos)  
-2. El conjunto de datos recopilado debería de tener entre 30 and 100 observaciones (filas) y de 5 a 10 características (columnas)  
-3. Podría enriquecer el conjunto de datos con más información obtenida con otros métodos además del tecleo manual (por ejemplo, web scraping)  
-4. Necesidad de completar un análisis para responder las preguntas que tenía que resolver con este proyecto. También debería complementar el análisis con algún tipo de hipótesis.  
-##### Mi proyecto  
-Mis preguntas eran sobre las leras de las canciones que solemos escuchar cada día, estas preguntas son:  
-1. ¿Las letras de las canciones tienen un sentimiento positivo en general?  
-2. ¿Son las letras de las mujeres más positivas que las de los hombres?  
-3. ¿Son las letras de las canciones pop más positivas que las de hip hop?  
-&lt;img&gt;image1&lt;/img&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">##### Mi solución
-###### Python  
-- Creación del conjunto de datos usando python:  
-Decidí recopilar la información desde [Spotify Charts](https://charts.spotify.com/) porque quería analizar letras de canciones globales, así que escogí el top de artistas de la semana 47 del año 2022. El proceso que seguí fue teclear en un fichero los artistas de esa lista y además también usé [Last.fm](https://www.last.fm/) para recopilar y teclear más información como género, género musical general y si era una banda o grupo.  
-Entonces completé el conjunto de datos buscando las 10 canciones más populares de cada artista en [Spotify](https://open.spotify.com/) usando su API.  
-Después usé la librería de [__lyricsgenius__](https://pypi.org/project/lyricsgenius/) para conectar al sitio web de [Genius](https://genius.com/) para descargar 5 de las 10 canciones recopiladas in Spotify of every artist (porque el nombre de las canciones en Spotify no siempre tenía correspondencia en el nombre dado en Genius).  
-En este momento también creé una función con [Selenium](https://www.selenium.dev/) para obtener el token de conexión, por si acaso el tocken the conexión a Genius cambiaba.  
-Ahora mismo está almacenado en un fichero (secrets.txt) pero podría obtenerlo sin almacenarlo.
-&lt;img&gt;image2&lt;/img&gt; 
-- Análisis de sentimiento:  
-Una vez que descargué toda la información, necesité tratarla para realizar el análisis de sentimiento (using the library [__Flair__](https://github.com/flairNLP/flair)) y procesamiento de lenguaje natural ([__NLTK__](https://www.nltk.org/)).
-- Traducciones:  
-Puesto que la lista de canciones estaban cantadas en diferentes lenguajes, decidí traducir todo a inglés para simplificar el análisis. Para realizar esto usé la librería [__Fasttext__](https://fasttext.cc/) con su modelo pre-entrenado para detectar el idioma de las letras y entonces traducirlas a inglés con la librería [__translators__](https://github.com/uliontse/translators) la cual si no puede hacer la traducción, usa el traductor de Google para realizar el trabajo.
-- Top palabras:  
-Calculé el top de palabras con las funciones de NLTK y actualicé manualmente las palabras prohibidas de la lista para incluir más de las que no me interesaban en mi análisis.
-- Nube de palabras:  
-También creé una función para generar una nube de palabras con las librerías __wordcloud__ y __PIL__ para mostrar diferentes silueta que he descargado.
-- Análisis de hipótesis:  
-En otro documento de Jupyter, desarrolé el análisis de hipótesis y preparé el conjunto de datos para el análisis visual con [Tableau](https://public.tableau.com/)
-###### Tableau  
-Usé la versión públicva de Tableau para crear la presentación del proyecto y el análisis visual, lo puedes encontrar en [_mi Tableau_](https://public.tableau.com/app/profile/.scar.iglesias.roqueiro/viz/Mid-BootcampProject_16711135428210/Lyrics)  
-&lt;img&gt;image3&lt;/img&gt;
-###### Flask  
-El proyecto incluye una demo en Flask que permite la búsqueda de una canción de un artista y mostrará la letra con el top de palabras traducidas, el análisis de sentimiento y una nube de palabras.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Para resumir los enlaces de mi proyecto, aquí están:  
-- Video de presentación: [__Mi Youtube__](https://youtu.be/Veu5M7_hCUg)  
-- Visualizaciones: [__Mi Tableau__](https://public.tableau.com/app/profile/.scar.iglesias.roqueiro/viz/Mid-BootcampProject_16711135428210/Lyrics)  
-- Código fuente (incluida la demo en Flask): [__Mi Github__](https://github.com/oiroqueiro/mid-bootcamp-project)  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">tableau, visualización, dashboard, python, flask, web scrapping, API, Selenium, análisis de sentimiento, traducción, repository</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IHRepo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Intelligent Helper Repository is my attempt to show how artificial intelligence can help in access to education.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This is the project that I created for my Final Bootcamp project in Data Analytics in [IronHack](http://www.ironhack.com). The idea was to try to improve the Bootcamp experience, acquiring more students and helping the existing students. So I decided to transcribe all the videos of my boot camp, translate all the texts (to Spanish at least but some to Portuguese, Italian, German, Chinese, and Hindi, as the languages that could speak my fantastic cohort), caption them, creating a summary and keywords, all automatic (at this moment, couldn't finish all the automatism but exists all the functions for that).     
-&lt;img&gt;image1&lt;/img&gt;    
-The project also includes one app to search and find videos about one topic (or any word you want to use in any language that was translated) and when decide on the video you want to explore have the option to search inside the video and locate the exact moment where the video talk about your searching (Future feature, continue the implementing of the FULL TEXT index in MySQL with the option of Natural Language).   
-To play the videos with subtitles and locate in the exact position I used [VLC media player](https://www.videolan.org/vlc/index.es.html).   
-I would wanted to train my models but my hardware and the time made me change my mind, however, this project is not closed so maybe in the future I return here to improve it.    
-&lt;img&gt;image2&lt;/img&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">##### Process    
-- **Transcription**   
-For this task, I decided to use [Whisper](https://github.com/openai/whisper). After testing different options, this was which fitted more to my project. I used the model "base.en" because of my schedule (I had to create the project after work) and hardware requirements but can use others larger to get better performance, or even multi-language.   
-- **Subtitles**   I had many problems managing the subtitles, I tried to split the videos but synchronizing again the subtitles was impossible with the time I had to do it, so in the end I decided to use [Stable Whisper](https://github.com/jianfch/stable-ts) without split the video.   
-- **Summary**   For this task, I decided to use [Hugging Face transformers](https://huggingface.co/docs/transformers/index) after trying other options, I also tried many different models and decided to use [**mrm8488/flan-t5-large-finetuned-openai-summarize_from_feedback**](https://huggingface.co/mrm8488/flan-t5-large-finetuned-gsm8k) which gave me better results.   
-- **Keywords**   [**KeyBERT**](https://maartengr.github.io/KeyBERT/) was the chosen between some alternatives and the model I used was [**universal-sentence-encoder**](https://tfhub.dev/google/universal-sentence-encoder/4)   
-- **Translation**   This was the only part that didn't try other options because I used it before and worked fine for me but this also was not a smooth path, &lt;u&gt; Beware that translating subtitles can give you some surprises (break lines...)&lt;/u&gt; so I decided to split the subtitles into lines and translate them to joined together at the end.   
-- **BBDD**   
-This process stores in one [__MySQL__](https://www.mysql.com/) database all the texts I got (originals and translations) with the relationship with the videos. I created a FULL-TEXT index in the database so I could use the natural language option to search the videos.   
-- **APP**   Since I tried Flask in my [__Lyrics__](https://github.com/oiroqueiro/mid-bootcamp-project) project, for this project I wanted to try other options and after researching Streamlit and Django, I decided to take the complicated path, so I used [__Django__](https://www.djangoproject.com/) (with [__Bootstrap 5__](https://getbootstrap.com/)).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;img&gt;image3&lt;/img&gt;
-As I said before, the limited time didn't allowed me to finish everything I had in my mind (launch all the logic from Django, update videos, option to transcribe online videos (at the moment only can use files).  But I think in this project there are a lot of information about this complicated path I had chosen.
-To summarize the links of my project, here they are:  
-- Presentation video: [__My Youtube__](https://youtu.be/mbKBJYidxc4)  
-- Hackshow video: [__My Youtube__](https://youtu.be/Veu5M7_hCUg)  
-- Source codes (including the Django App): [__My Github__](https://github.com/oiroqueiro/final-project-bootcamp)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python, django, mysql, bbdd, trasnscription, subtitles, summary, keywords, translation, repository, video</t>
-  </si>
-  <si>
-    <t xml:space="preserve">project0301</t>
-  </si>
-  <si>
-    <t xml:space="preserve">project0302</t>
-  </si>
-  <si>
-    <t xml:space="preserve">project0303</t>
-  </si>
-  <si>
-    <t xml:space="preserve">project0304</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Intelligent Helper Repository (Ayudante Inteligente de Respositorio) es mi intento por mostrar como la inteligencia artificial puede ayudar en el acceso a la educación.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Este es el proyecto que creé para mi tarea de final de Bootcamp en el curso de Análisis de Datos en [IronHack](http://www.ironhack.com). La idea era intentar mejorar la experiencia del Bootcamp, adquiriendo más estudiantes y ayudando a los existentes. Así que decidí transcribir todos los videos de mi bootcamp, traduciendo todos los textos (a español por lo menos pero alguno también a portugué, italiano, alemán, chino e hindi, como los idiomas que mi fantásticos compañeros y profesores podían hablar), suntitulando, creando resúmenes del contenido y palabras clave, todo automatizado (en este momento, no pude terminar todos los automatismos pero existen todas las funciones para ello).  
-&lt;img&gt;image1&lt;/img&gt;
-El proyecto también incluye una aplicación para buscar y encontrar videos que hablen sobre un tema (o cualquier palabra que se quiera buscar en cualquiera de los idiomas en que están traducidos los videos) y cuando se encuentra el video que se desea explorar, da la opción de hacer una búsqueda dentro del video y localizar el momento exacto donde se habla sobre lo que se está buscando (futura característica, continuar implementando los índices FULL TEXT en MySQL con la opción de Lenguaje Natural).  
-Para reproducir los videos con subtitulos y localizar la posición exacta he usado [VLC media player](https://www.videolan.org/vlc/index.es.html).  
-Me gustaría poder entrenar mis propios modelos pero el hardware de mi pc y el tiempo me hicieron desistir, sin embargo el proyecto no está cerrado y quizás en un futuro puedo volver a él para mejorarlo.
-&lt;img&gt;image2&lt;/img&gt;</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">##### Proceso   
-- **Transcripción**  
-Para esta tarea decidí usar [Whisper](https://github.com/openai/whisper). Después de probar diferentes opciones, esta fue la que se ajustaba mejor a mi proyecto. Usé el modelo "base.en" debido a mi calendario (tengo un trabajo a tiempo completo, con lo que el proyecto tenía que desarrollarlo después de mi trabajo) y los requerimientos de hardwaree requirements pero se puede usar otro modelo más pesado para obtener mejor resultado, o incluso multi-idioma.  
-- **Subtítulos**  
-Tuve muchos problemas para gestionar los subtítulos, Intenté partir los videos pero el sincronizarlos de nuevo se volvió imposible con el tiempo que tenía para hacerlo, así que al final decidí usar [Stable Whisper](https://github.com/jianfch/stable-ts) sin partir los videos.  
-- **Resumir**  
-Para esta tarea decidí usar [Hugging Face transformers](https://huggingface.co/docs/transformers/index) después de probar otras opciones, también probé varios modelos distintos y al final decidí usar [**mrm8488/flan-t5-large-finetuned-openai-summarize_from_feedback**](https://huggingface.co/mrm8488/flan-t5-large-finetuned-gsm8k) el cual me dio los mejores resultados.  
-- **Palabras clave**  
-[**KeyBERT**](https://maartengr.github.io/KeyBERT/) fue la opción escogida entre varias alternativas y el the model que usé fue [**universal-sentence-encoder**](https://tfhub.dev/google/universal-sentence-encoder/4)  
-- **Traducción**  
-Esta fue la única parte en la que no probé alternativas porque lo había utilizado anteriormente en mi proyecto Lyrics y funcionó perfectamente para mi aunque no fue un camino de rosas, &lt;u&gt;cuidado al traducir subtítulos ya que te pueden dar algunas sorpresas (saltos de líneas...)&lt;/u&gt; así que decidí partir los subtítulos en líneas, traducirlas y unirlas luego todas juntas al final.  
-- **Base de datos**  
-En este proceso guardé en una base de datos [__MySQL__](https://www.mysql.com/) todos los textos que tenía (originales y traducciones) con su relación con los videos. Creé un índice FULL TEXT en la base de datos por lo que pude usar la opción de búsqueda con lenguaje natural para buscar los videos.  
-- **Aplicación**  
-Ya que usé Flask en mi proyecto [__Lyrics__](https://github.com/oiroqueiro/mid-bootcamp-project) project, para este proyecto quería intentar alguna otra opción y después de investigar sobre Streamlit y Django, decidí tomar el camino más complicado, así que usé [__Django__](https://www.djangoproject.com/) (con [__Bootstrap 5__](</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">https://getbootstrap.com</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">/)).</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;img&gt;image3&lt;/img&gt;
-Como dije anteriormente, el límite de tiempo no me permitó terminar todo lo que tenía en mi cabeza (lanzar la lógica desde Django, actualizar videos, opción de transcribir videos online -de momento solo pude usar ficheros en local-).  Pero pienso que en este proyecto hay un montón de información sobre esta complicada travesía que escogí.
-Para resumir los enlaces de mi proyecto, aquí están:  
-- Video de presentación: [__My Youtube__](https://youtu.be/mbKBJYidxc4)  
-- Video en el Hackshow: [__My Youtube__](https://youtu.be/Veu5M7_hCUg)  
-- Código fuente (incluida la aplicación de Django): [__My Github__](https://github.com/oiroqueiro/final-project-bootcamp)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python, django, mysql, base de datos, transcripción, subtítulos, resumen, palabras clave, traducción, repositorio, video</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Portfolio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Portfolio built from scratch, from website planning with no idea of web development to deployment with docker without idea of containers.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I had several projects that I wanted to show but I didn't like the idea of using one existent website because all the alternatives that I was trying didn't have some of the features I thought were a must in my portfolio or were not flexible to customize it or were not beautiful (or what I consider beautiful for a portfolio).  
-Using one of those platforms would be the best option since I have a full-time job and two little girls born during the pandemic years, but I decided to go for it through the complicated path (sometimes hell path) and &lt;u&gt;create my portfolio from scratch&lt;/u&gt;.  
-I know that one portfolio is not a good example for a data analytics project, actually is not related to data analytics, but this project was a great opportunity to show my determination, creative problem solving, adaptability and to learn a lot along the time I would dedicate to this project.  
-The features I wanted in my portfolio include:  
-1. Multi-language  
-2. Responsive website  
-3. Light/Dark mode  
-4. Customizable
-5. Containerized  
-6. Index Search  
-The first four were mandatory, the other two I wanted to learn and practice.  
-So let's explain the path from the beginning.  
-&lt;img&gt;image1&lt;/img&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#### **The path**  
-Since I am not a UX/Designer or web developer, and my knowledge of HTML, CSS, and JavaScript was limited, the challenge started being super hard for me.   
-##### **Multi-language**  
-One thing that I was sure would not happen was the use of a library to translate all the texts automatically. I know that there are fantastic options out there that could make my portfolio accessible to almost everyone, but I think that a feature made like this would run against the nature of one portfolio.  
-A portfolio should be a presentation card of the work of someone to show the skills of the owner, using an automated tool, which is quite easy to implement (I know what I'm talking about because I used it in 2 of my previous projects and of course, I am not against this), is not what I wanted, so the choice I took to implement the multi-language was translated by myself the texts and store them in the database making easy to the users to change between the languages that the owner knows (or decide to show).  
-##### **The website**  
-When I started to investigate my options to create one website, the beginning was very discouraging. Only when I discovered [**Hugo**](https://gohugo.io/) I started to see the light at the end of the tunnel. Hugo is a framework for building websites with a lot of beautiful templates for websites and a great community. So I was researching Hugo and his templates for quite a while until I found some templates that could fit my requirements. The problem was that Hugo is fantastic for building static websites which is the opposite of my idea of one portfolio.  
-So in the end when I chose the [**iWriter**](https://github.com/statichunt/iwriter-hugo) template arrived at the moment to adapt it to a dynamic website.  
-##### **Flask**  
-One technology that I wanted to explore and improve my skills in was [**Python**](https://www.python.org/) because has tons of libraries, frameworks, and an impressive community behind it. So, when I thought about dynamic websites, [**Flask**](https://flask.palletsprojects.com/en/3.0.x/) came quickly to my mind. Since I worked with it in my [*Lyrics*](https://github.com/oiroqueiro/mid-bootcamp-project) project, I knew about his capabilities but the hard work had just started.  
-I had to adapt the iWriter template to be a dynamic template with [Jinja](https://jinja.palletsprojects.com/en/3.1.x/templates/) without losing any functionality I liked about this template.  
-After spending many, many, many hours understanding the HTML, CSS, javascript, and Bootstrap (and other technologies) that my template was used to have such features and more hours cleaning the code and adapting, I had some templates quite cleaned and ready to use with the logic of my website.  
-At this point I want to share with all of you [**this fantastic tutorial of Flask**](https://blog.miguelgrinberg.com/post/the-flask-mega-tutorial-part-i-hello-world), by *Miguel Grinberg*. I also use this one, in Spanish, of [**j2logo**](https://j2logo.com/tutorial-flask-espanol/) by *Juan José Lozano Gómez*. I learned a lot with them and with all the features that I had to face.  
-&lt;img&gt;image2&lt;/img&gt;
-##### **Customizable**  
-I wanted a customizable website so after evaluating different options, I decided to use one Excel file to store all the texts of my website in addition to the content of my portfolio. The menus texts, buttons, images, ... can be adapted easily.  
-At the beginning I thought to manage the creation of the content within the website, but soon I realized that I didn't have time if I wanted to finish the project this year. Nevertheless, I did investigate and in the end, I could create one part that makes me feel a little proud of, it is that I could make the URLs to the login and logout pages of my website customizable via environment variables. The option of editing the content would be a future feature.  
-And how could I make the content of my portfolio customizable? Firstly I thought about the use of HTML, then the use of [**Markdown**](https://www.markdownguide.org/), and in the end, I thought what's better than allowing the use of both? So, we can write our content using Markdown and HTML labels and use both at the same time.  
-##### **DDBB**  
-I have been working with Microsoft SQL Server for more than 15 years and lately, I have been working with MySQL, at the beginning of my career I was using for years Oracle. So for this project, I decided to try a new one and the choice for developing was [**SQLite**](https://www.sqlite.org/index.html) but to use it in production once I deploy the project I went for [**PostgreSQL**](https://www.postgresql.org/). The good part is that the portfolio works perfectly with both so only changing the environment variables can use SQLite, PostgreSQL, or another different.  
-##### **The search**  
-In the beginning, my portfolio would have very few projects, so a searching function would not be too important but I wanted to create one project alive for a long time and easily maintainable so in the end I implemented a simple search function using the queries of the extension [**FlaskSQLAlchemy**](https://flask-sqlalchemy.palletsprojects.com/en/3.1.x/) which was the library that I was using to work with the databases. But in the last months I have been reading quite often about NoSQL databases, and the capabilities of [**Elasticsearch**](https://www.elastic.co/) for searching, so I decided to start working with this kind of databases using Elasticsearch in my project.  
-Finally, the option of search in my portfolio is powered by Elasticsearch and, in case this engine is not present in our enviroment, will be powered by FlaskSQLAlchemy.  
-I also have a search of keywords, this is much simpler and it will find only the keyword we are searching but with the characteristic of bringing the keywords that share the projects where our keyword search is present too.  
-##### **Containerization**  
-And, if all the technologies I had to explore, learn, and implement for my project were not enough, I decided that I should containerize my app. So I started to learn [**Docker**](https://www.docker.com/) since this is one of the most popular platforms. During my learning path, I was able to create a docker container with my Flask app, so I had one docker container with my portfolio working but I wanted to create all my whole project with containers. In the end, I finished with a docker network with 3 containers:   
-- The first one, and more important because has all the data, one PostgreSQL docker 
-- The second one, if present, is the Elasticsearch docker for the searching functionality 
-- The third one is my Flask app which has even the HTTP Server powered by [**Gunicorn**](https://gunicorn.org/)  
-##### **Deployment**  
-(I am still working on this part)  
-As the last step of my project, I need to deploy it. During this path, I was working always with opensource or free-of-charge options (except the domain name that I had to pay) and the option I found that could work for me was the use of [**OCI**](https://www.oracle.com/es/cloud/), the **Oracle Cloud Infrastructure** that has one Free Tier (Always Free Services) which I could use for the deployment.  
-In addition to this, I created one [**Google Analytics**](https://analytics.google.com/) account to monitor and analyze my website.  
-&lt;img&gt;image3&lt;/img&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">To summarize, the links of this project are:  
-- All the source code (including the docker and compose files): [**My Github**](https://github.com/oiroqueiro/portfolio)  
-- Live demo: [**my Portfolio Website**](http://www.oscarlytics.com)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python, flask, hugo, sqlite, postgresql, elasticsearch, container, docker, multi-language, portfolio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">project0401</t>
-  </si>
-  <si>
-    <t xml:space="preserve">project0402</t>
-  </si>
-  <si>
-    <t xml:space="preserve">project0403</t>
-  </si>
-  <si>
-    <t xml:space="preserve">project0404</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Portafolio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Portafolio creado desde cero, desde la planificación de la página web sin saber desarrollo web hasta la implementación con Docker sin tener idea de contenedores.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tenía varios proyectos que quería mostrar pero no me gustaba la idea de user una página web existente porque todas las alternativas que había probado no tenían todas las caracterías que pensaba eran necesarias en mi portafolio o no eran flexibles para personalizarlas o no eran suficientemene bonitas (o lo que yo considero bonito para un portafolio).  
-Usar una de esas plataformas sería la mejor opción ya que tengo un trabajo a jornada completa y dos pequeñas nacidas durante los años de la pandemia, pero decidí tomar el camino más complicado (a veces infernal) y &lt;u&gt;crear mi portafolio desde cero&lt;/u&gt;.  
-Sé que un portafolio no es un gran ejemplo como proyecto de análisis de datos, realmente no está relacionado con el análisis de datos, pero sí que es una gran oportunidad para mostrar mi determinación, resolución creativa de problemas, adaptabilidad y aprender un montón durante todo el tiempo que le he dedicado a este proyecto.  
-Las características que me gustaría que tuviera mi portafolio incluyen:  
-1. Multi-idioma  
-2. Página web adaptable (responsive)  
-3. Modo claro/oscuro  
-4. Personalizable  
-5. Uso de contenedores  
-6. Búsqueda por índices  
-Las primeras 4 eran obligatorias, las otras dos me gustaría aprenderlas y practicar con ellas  
-Así que paso a explicar el camino desde el principio.  
-&lt;img&gt;image1&lt;/img&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#### **El camino**  
-Puesto que yo no soy un diseañador o desarrollador web, y mi conocimiento de HTML, CSS, y JavaScript era limitado, el reto empezó siendo super complicado para mi..   
-##### **Multi-idioma**  
-Una cosa de la que yo estaba seguro que no iba a pasar era el uso de una librería para realizar la traducción de todos los textos automáticamente. Sé que hay fantásticas opciones por ahí que podrían hacer mi portafolio accesible a casi todo el mundo, pero creo que una característica como esta iría contra lo que es la naturaleza de un portafolio.  
-Un portafolio debería de ser una carta de presentación del trabajo de alguien para mostrar las habilidades del propietario, el uso de una herramienta automatizada, la cual es bastante sencilla de implementar (sé de lo que hablo porque la usé en 2 de mis anteriores proyectos y por supuesto, no estoy en contra de su uso), no es lo que yo quería, así que la opción que escogí para implementar el multi-idioma fue traducir por mí mismo los textos y guardarlos en la base de datos haciendo sencillo para los usuarios su uso y el cambio entre los idiomas que el dueño conoce (o decide mostrar).  
-##### **La página web**  
-Cuando empecé a investigar mis opciones de crear una página web, el inicio fue descorazonador. Solamente cuando descubrí [**Hugo**](https://gohugo.io/) empecé a ver la luz al final del túnel. Hugo es una plataforma para construir sitios web con muchas plantillas bonitas y una gran comunidad. Así que estuve investigando Hugo y sus plantillas bastante tiempo hasta que encontŕé algunas que podrían cumplir con mis requerimientos. El problema era que Hugo es fantástico para crearr páginas web estáticas lo que es contrario a mi idea de un portafolio.  
-De manera que al final cuando escogí la plantilla de [**iWriter**](https://github.com/statichunt/iwriter-hugo) llegó el momento de adaptarla a un sitio web dinámico.  
-##### **Flask**  
-Una tecnología que quería explorar y en la que quería mejorar mis habilidades era [**Python**](https://www.python.org/) porque tiene cientos de librerías, frameworks, y con una impresionante comunidad detrás. Así, cuando pensé en sitios web dinámicos, [**Flask**](https://flask.palletsprojects.com/en/3.0.x/) vino rápidamente a mi mente. Desde que había trabajado con él en mi proyecto [*Lyrics*](https://github.com/oiroqueiro/mid-bootcamp-project), conocía sus capacidades pero la parte dura del trabajo no solamente acababa de empezar.  
-Tuve que adaptar la plantilla iWriter para ser una plantilla dinámica con [Jinja](https://jinja.palletsprojects.com/en/3.1.x/templates/) sin perder ninguna funcionalidad que me gustaba de esta plantilla.  
-Después de invertir muchas, muchas, mychas horas entendiendo el HTML, CSS, JavaScript, y Bootstrap (y otras tecnología) que mi plantilla estaba usando para tener tales funcionalidades y más horas limpiando el código y adaptándolo, conseguí tener algunas plantillas bastante limpias y listas para usar con la lógica de mi página web.  
-En este punto quería compartir con todos vosotros [**este fantástico tutorial de Flask**](https://blog.miguelgrinberg.com/post/the-flask-mega-tutorial-part-i-hello-world), de *Miguel Grinberg*. También usé este otro, en Español, de [**j2logo**](https://j2logo.com/tutorial-flask-espanol/) por *Juan José Lozano Gómez*. Aprendí un montón con ellos y con todas las funcionalidades que tuve que encarar.  
-&lt;img&gt;image2&lt;/img&gt;
-##### **Personalizable**  
-Quería una página web personalizable así que después de evaluar diferentes opciones, decidí usar un fichero Excel para almacenar los textos de mi sitio web junto con el contenido de mi portafolio. Los textos de los menús, botones, imagenes, .. pueden ser adaptadas facilmente.  
-Al principio pensé en gestionar la creación del contenido desde el propio sitio web, pero pronto me di cuenta de que no tenía tiempo si quería terminar el proyecto este año. Sin embargo, investigué y al final,  pude crear una parte de la que me siento un poco orgulloso, esto es que pude hacer las URLs para las páginas de inicio de sesión y fin de sesión de mi sitio web personalizadas via variables de entorno. La opción de editar el contenido sería una funcionalidad para el futuro.  
-Y cómo podría hacer el contenido de mi portafolio personalizable? Primero pensé en el uso de HTML, después en el uso de [**Markdown**](https://www.markdownguide.org/), y al final, pendé, ¿qué es mejor que permitir el uso de ambos? Así, podemos escribir nuestro contenido usando etiquetas Markdown y HTML al mismo tiempo.  
-##### **BBDD**  
-He trabajado con Microsoft SQL Server durante más de 15 years and últimamente, he estado trabajando con MySQL, al principio de mi carrera estuve usando Oracle durante años. Así que para este proyecto, decidí intentar una nueva base de dtaos y la opción escogida para desarrollo era [**SQLite**](https://www.sqlite.org/index.html) pero para el uso en producción una vez implementara el proyecto sería [**PostgreSQL**](https://www.postgresql.org/). La mejor parte es que mi portafolio funciona perfectamente con  ambas así que solamente hay que cambiar las variables de entorno para usar SQLite, PostgreSQL, u otra base de datos distinta.  
-##### **La búsqueda**  
-Al principio, mi portafolio tendría pocos proyectos, así que una funcionalidad de búsqueda no sería demasiado importante pero quería crear un proyecto vivo durante bastante tiempo y facilmente mantenible así que al final implementé una función sencilla de búsqueda usando las consultas de la extensión [**FlaskSQLAlchemy**](https://flask-sqlalchemy.palletsprojects.com/en/3.1.x/) la cual era la librería que estaba usando para trabajar con las bases de datos. Pero los últimos meses he estado leyendo bastante a menudo sobre bases de datos NoSQL, y las capacidades de [**Elasticsearch**](https://www.elastic.co/) para la búsqueda, así que decidí empezar a trabajar con este tipo de bases de datos usando Elasticsearch en mi proyecto.  
-Finalmente, la opción de búsqueda en mi portafolio está facilitada por Elasticsearch y, en caso de que esta herramienta no está presente en nuestro entorno, será gestionada por FlaskSQLAlchemy.  
-También tengo una búsqueda de palabras clave, esta es mucho más simple y encontrará solamente la palabra clave que estemos buscando pero con la característica de traer también las palabras claves que comparten los proyectos donde nuestra palabra clave de búsqueda esté presente.  
-##### **Contenedores**  
-Y, si no fuera suficiente con todas las tecnologías que tuve que explorar, aprender, e implementar para mi proyecto, decidí que debería usar contenedores en mi aplicación. Así que empecé a aprender [**Docker**](https://www.docker.com/) ya que es una de las plataformas más populares. Durante mi aprendizaje, fue capaz de crear un contenedor de docker para mi aplicación Flask, así que tenía un contenedor docker con mi portafolio funcionando pero quería crear todo mi proyecto con contenedores. Al final, terminé con una red de docker con 3 contenedores:   
-- El primero, y más importante porque tiene todo los datos, un docker con PostgreSQL 
-- El segundo, si está presente, es el docker de Elasticsearch para la funcionalidad de búsquedas 
-- El tercero es mi aplicación Flask la cual tiene incluso el servidor HTTP gestionado con [**Gunicorn**](https://gunicorn.org/)  
-##### **Implementación**  
-(Todavía estoy con esta parte)  
-Como último paso de mi proyecto, necesito implementarlo. Durante toda esta ruta, estuve trabajando siempre con opensource u opciones gratuitas (excepto el nombre de dominio que he tenido que pagar) y la opción que he encontrado y que podría funcionar para mi era el uso de [**OCI**](https://www.oracle.com/es/cloud/), la **Infraestructura de la nube de Oracle** (Oracle Cloud Infrastructure) que tenía una opción gratuita (Always Free Services) la cual podría usar para la implementación.  
-Además, creé una cuenta de [**Google Analytics**](https://analytics.google.com/) para controlar y analizar mi página web.  
-&lt;img&gt;image3&lt;/img&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resumendo, los enlaces de mi proyecto son:  
-- Todo el código fuente (incluyendo los ficheros docker y docker compose): [**My Github**](https://github.com/oiroqueiro/portfolio)  
-- Demo real: [**my Portfolio Website**](http://www.oscarlytics.com)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python, flask, hugo, sqlite, postgresql, elasticsearch, contenedor, docker, multi-idioma, portafolio</t>
   </si>
 </sst>
 </file>
@@ -1211,7 +707,7 @@
   <dimension ref="A1:D57"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="D53" activeCellId="0" sqref="D53"/>
     </sheetView>
@@ -1879,9 +1375,9 @@
   <dimension ref="A1:D47"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+      <selection pane="bottomLeft" activeCell="D39" activeCellId="0" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1929,23 +1425,18 @@
       <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>93</v>
-      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>89</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="10" t="s">
-        <v>95</v>
-      </c>
+      <c r="D4" s="10"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
@@ -1958,7 +1449,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1971,27 +1462,22 @@
       <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>93</v>
-      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>89</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="10" t="s">
-        <v>97</v>
-      </c>
+      <c r="D7" s="10"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>90</v>
@@ -1999,86 +1485,74 @@
       <c r="C8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="10" t="s">
-        <v>99</v>
-      </c>
+      <c r="D8" s="10"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="10" t="s">
-        <v>101</v>
-      </c>
+      <c r="D9" s="10"/>
     </row>
     <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="10" t="s">
-        <v>103</v>
-      </c>
+      <c r="D10" s="10"/>
     </row>
     <row r="11" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>104</v>
-      </c>
       <c r="C11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="11" t="s">
-        <v>105</v>
-      </c>
+      <c r="D11" s="11"/>
     </row>
     <row r="12" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="10" t="s">
-        <v>107</v>
-      </c>
+      <c r="D12" s="10"/>
     </row>
     <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="10" t="s">
-        <v>109</v>
-      </c>
+      <c r="D13" s="10"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>1</v>
@@ -2086,77 +1560,69 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D16" s="10" t="s">
-        <v>114</v>
-      </c>
+      <c r="D16" s="10"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D17" s="10" t="s">
-        <v>116</v>
-      </c>
+      <c r="D17" s="10"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D18" s="10" t="s">
-        <v>118</v>
-      </c>
+      <c r="D18" s="10"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D19" s="11" t="s">
-        <v>120</v>
-      </c>
+      <c r="D19" s="11"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>90</v>
@@ -2164,86 +1630,74 @@
       <c r="C20" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D20" s="10" t="s">
-        <v>121</v>
-      </c>
+      <c r="D20" s="10"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D21" s="10" t="s">
-        <v>122</v>
-      </c>
+      <c r="D21" s="10"/>
     </row>
     <row r="22" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D22" s="10" t="s">
-        <v>123</v>
-      </c>
+      <c r="D22" s="10"/>
     </row>
     <row r="23" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>104</v>
-      </c>
       <c r="C23" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D23" s="10" t="s">
-        <v>124</v>
-      </c>
+      <c r="D23" s="10"/>
     </row>
     <row r="24" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D24" s="10" t="s">
-        <v>125</v>
-      </c>
+      <c r="D24" s="10"/>
     </row>
     <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D25" s="10" t="s">
-        <v>126</v>
-      </c>
+      <c r="D25" s="10"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>2</v>
@@ -2251,304 +1705,287 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D28" s="10" t="s">
-        <v>128</v>
-      </c>
+      <c r="D28" s="10"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D29" s="10" t="s">
-        <v>129</v>
-      </c>
+      <c r="D29" s="10"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D30" s="10" t="s">
-        <v>130</v>
-      </c>
+      <c r="D30" s="10"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D31" s="11" t="s">
-        <v>120</v>
-      </c>
+      <c r="D31" s="11"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>132</v>
+        <v>110</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>133</v>
+        <v>111</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>134</v>
+        <v>112</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>135</v>
+        <v>113</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>136</v>
+        <v>114</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>138</v>
+        <v>116</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>139</v>
+        <v>117</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>140</v>
+        <v>118</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>142</v>
+        <v>120</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>143</v>
+        <v>121</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>145</v>
+        <v>123</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D39" s="10" t="s">
-        <v>146</v>
-      </c>
+      <c r="D39" s="10"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>132</v>
+        <v>110</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>147</v>
+        <v>124</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D41" s="10" t="s">
-        <v>148</v>
+        <v>125</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>135</v>
+        <v>113</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>149</v>
+        <v>126</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D43" s="10" t="s">
-        <v>150</v>
+        <v>127</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>139</v>
+        <v>117</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>151</v>
+        <v>128</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D45" s="10" t="s">
-        <v>152</v>
+        <v>129</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>143</v>
+        <v>121</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D46" s="10" t="s">
-        <v>153</v>
+        <v>130</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>145</v>
+        <v>123</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D47" s="10" t="s">
-        <v>154</v>
-      </c>
+      <c r="D47" s="10"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D11" r:id="rId1" display="Then, when my youngest baby was ready to be born I had the chance to join [**Ironhack**](https://www.ironhack.com/es/en/data-analytics/remote) to improve my skills of data mining and learn much more about analysis and artificial intelligence. &#10;During this time I had to face many challenges that the teaching team provided us which I could solve, making me feel more confident with my skills and learning and creating projects (like my final project, Ironhack repository) that could help others to improve their skills too.&#10;"/>
-    <hyperlink ref="D19" r:id="rId2" display="https://www.youtube.com/embed/8CAoLz4NS5o"/>
-    <hyperlink ref="D31" r:id="rId3" display="https://www.youtube.com/embed/8CAoLz4NS5o"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -2566,10 +2003,10 @@
   </sheetPr>
   <dimension ref="A1:X9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
-      <selection pane="bottomLeft" activeCell="R9" activeCellId="0" sqref="R9"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2587,58 +2024,58 @@
   <sheetData>
     <row r="1" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>155</v>
+        <v>131</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>156</v>
+        <v>132</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>132</v>
+        <v>110</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>157</v>
+        <v>133</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>158</v>
+        <v>134</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>159</v>
+        <v>135</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>160</v>
+        <v>136</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>161</v>
+        <v>137</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>163</v>
+        <v>139</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>164</v>
+        <v>140</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>165</v>
+        <v>141</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>166</v>
+        <v>142</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>167</v>
+        <v>143</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>168</v>
+        <v>144</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>170</v>
+        <v>146</v>
       </c>
       <c r="S1" s="2"/>
       <c r="T1" s="2"/>
@@ -2648,339 +2085,77 @@
       <c r="X1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="13" t="n">
-        <v>44890</v>
-      </c>
-      <c r="B2" s="12" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="H2" s="14" t="s">
-        <v>175</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="P2" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>179</v>
-      </c>
+      <c r="A2" s="13"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="14"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="13" t="n">
-        <v>44890</v>
-      </c>
-      <c r="B3" s="12" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="H3" s="14" t="s">
-        <v>184</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="O3" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="P3" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>179</v>
-      </c>
+      <c r="A3" s="13"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="14"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="13" t="n">
-        <v>44912</v>
-      </c>
-      <c r="B4" s="12" t="n">
-        <v>1</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="H4" s="15" t="s">
-        <v>190</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="O4" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="P4" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>195</v>
-      </c>
+      <c r="A4" s="13"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="15"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="13" t="n">
-        <v>44912</v>
-      </c>
-      <c r="B5" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="G5" s="15" t="s">
-        <v>198</v>
-      </c>
-      <c r="H5" s="15" t="s">
-        <v>199</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="O5" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="P5" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="Q5" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="R5" s="1" t="s">
-        <v>195</v>
-      </c>
+      <c r="A5" s="13"/>
+      <c r="B5" s="8"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="13" t="n">
-        <v>44996</v>
-      </c>
-      <c r="B6" s="12" t="n">
-        <v>1</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="H6" s="15" t="s">
-        <v>205</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>206</v>
-      </c>
+      <c r="A6" s="13"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="15"/>
       <c r="L6" s="5"/>
-      <c r="O6" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="P6" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="Q6" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="R6" s="1" t="s">
-        <v>210</v>
-      </c>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="13" t="n">
-        <v>44996</v>
-      </c>
-      <c r="B7" s="12" t="n">
-        <v>1</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>215</v>
-      </c>
+      <c r="A7" s="13"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="4"/>
       <c r="L7" s="5"/>
-      <c r="O7" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="P7" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="Q7" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="R7" s="1" t="s">
-        <v>210</v>
-      </c>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="13" t="n">
-        <v>45287</v>
-      </c>
-      <c r="B8" s="12" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="F8" s="16" t="s">
-        <v>218</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>219</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>220</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="O8" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="P8" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="Q8" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="R8" s="5" t="s">
-        <v>225</v>
-      </c>
+      <c r="A8" s="13"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="13" t="n">
-        <v>45287</v>
-      </c>
-      <c r="B9" s="12" t="n">
-        <v>1</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>228</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="O9" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="P9" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="Q9" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="R9" s="5" t="s">
-        <v>225</v>
-      </c>
+      <c r="A9" s="13"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1" display="So, if you want to see the result of this project, you can go to [**One story about Life Expectancy**](https://public.tableau.com/views/TableauProject_16693794082020/Presentation?:language=en-US&amp;:display_count=n&amp;:origin=viz_share_link)"/>
-    <hyperlink ref="H3" r:id="rId2" display="Así que, si quieres ver el resultado de este proyecto, puedes ir a [**Una historia sobre Esperanza de Vida**](https://public.tableau.com/views/TableauProject_16693794082020/Presentation?:language=en-US&amp;:display_count=n&amp;:origin=viz_share_link)"/>
-    <hyperlink ref="H4" r:id="rId3" display="To summarize the links of my project, here they are:  &#10;&#10;- Presentation video: [__My Youtube__](https://youtu.be/Veu5M7_hCUg)  &#10;- Visualizations: [__My Tableau__](https://public.tableau.com/app/profile/.scar.iglesias.roqueiro/viz/Mid-BootcampProject_16711135428210/Lyrics)  &#10;- Source codes (including the Flask App): [__My Github__](https://github.com/oiroqueiro/mid-bootcamp-project)&#10;"/>
-    <hyperlink ref="G5" r:id="rId4" display="##### Mi solución&#10;  &#10;###### Python  &#10;  &#10;- Creación del conjunto de datos usando python:  &#10;Decidí recopilar la información desde [Spotify Charts](https://charts.spotify.com/) porque quería analizar letras de canciones globales, así que escogí el top de artistas de la semana 47 del año 2022. El proceso que seguí fue teclear en un fichero los artistas de esa lista y además también usé [Last.fm](https://www.last.fm/) para recopilar y teclear más información como género, género musical general y si era una banda o grupo.  &#10;Entonces completé el conjunto de datos buscando las 10 canciones más populares de cada artista en [Spotify](https://open.spotify.com/) usando su API.  &#10;Después usé la librería de [__lyricsgenius__](https://pypi.org/project/lyricsgenius/) para conectar al sitio web de [Genius](https://genius.com/) para descargar 5 de las 10 canciones recopiladas in Spotify of every artist (porque el nombre de las canciones en Spotify no siempre tenía correspondencia en el nombre dado en Genius).  &#10;En este momento también creé una función con [Selenium](https://www.selenium.dev/) para obtener el token de conexión, por si acaso el tocken the conexión a Genius cambiaba.  &#10;Ahora mismo está almacenado en un fichero (secrets.txt) pero podría obtenerlo sin almacenarlo.&#10;&lt;img&gt;image2&lt;/img&gt; &#10;- Análisis de sentimiento:  &#10;Una vez que descargué toda la información, necesité tratarla para realizar el análisis de sentimiento (using the library [__Flair__](https://github.com/flairNLP/flair)) y procesamiento de lenguaje natural ([__NLTK__](https://www.nltk.org/)).&#10;- Traducciones:  &#10;Puesto que la lista de canciones estaban cantadas en diferentes lenguajes, decidí traducir todo a inglés para simplificar el análisis. Para realizar esto usé la librería [__Fasttext__](https://fasttext.cc/) con su modelo pre-entrenado para detectar el idioma de las letras y entonces traducirlas a inglés con la librería [__translators__](https://github.com/uliontse/translators) la cual si no puede hacer la traducción, usa el traductor de Google para realizar el trabajo.&#10;- Top palabras:  &#10;Calculé el top de palabras con las funciones de NLTK y actualicé manualmente las palabras prohibidas de la lista para incluir más de las que no me interesaban en mi análisis.&#10;- Nube de palabras:  &#10;También creé una función para generar una nube de palabras con las librerías __wordcloud__ y __PIL__ para mostrar diferentes silueta que he descargado.&#10;- Análisis de hipótesis:  &#10;En otro documento de Jupyter, desarrolé el análisis de hipótesis y preparé el conjunto de datos para el análisis visual con [Tableau](https://public.tableau.com/)&#10;&#10;###### Tableau  &#10;Usé la versión públicva de Tableau para crear la presentación del proyecto y el análisis visual, lo puedes encontrar en [_mi Tableau_](https://public.tableau.com/app/profile/.scar.iglesias.roqueiro/viz/Mid-BootcampProject_16711135428210/Lyrics)  &#10;&#10;&lt;img&gt;image3&lt;/img&gt;&#10;&#10;###### Flask  &#10;El proyecto incluye una demo en Flask que permite la búsqueda de una canción de un artista y mostrará la letra con el top de palabras traducidas, el análisis de sentimiento y una nube de palabras."/>
-    <hyperlink ref="H5" r:id="rId5" display="Para resumir los enlaces de mi proyecto, aquí están:  &#10;&#10;- Video de presentación: [__Mi Youtube__](https://youtu.be/Veu5M7_hCUg)  &#10;- Visualizaciones: [__Mi Tableau__](https://public.tableau.com/app/profile/.scar.iglesias.roqueiro/viz/Mid-BootcampProject_16711135428210/Lyrics)  &#10;- Código fuente (incluida la demo en Flask): [__Mi Github__](https://github.com/oiroqueiro/mid-bootcamp-project)  "/>
-    <hyperlink ref="H6" r:id="rId6" display="&lt;img&gt;image3&lt;/img&gt;&#10;&#10;As I said before, the limited time didn't allowed me to finish everything I had in my mind (launch all the logic from Django, update videos, option to transcribe online videos (at the moment only can use files).  But I think in this project there are a lot of information about this complicated path I had chosen.&#10;&#10;To summarize the links of my project, here they are:  &#10;- Presentation video: [__My Youtube__](https://youtu.be/mbKBJYidxc4)  &#10;- Hackshow video: [__My Youtube__](https://youtu.be/Veu5M7_hCUg)  &#10;- Source codes (including the Django App): [__My Github__](https://github.com/oiroqueiro/final-project-bootcamp)"/>
-    <hyperlink ref="G7" r:id="rId7" display="https://getbootstrap.com"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>